<commit_message>
Results for 1a complete
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Semester1\Research\Smart-Grid-Blockchain-Privacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62464343-4FE9-4A53-8195-E0EEBC21B1C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DF2BF2-132E-4F27-938F-2C1A3F6F3857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15150" yWindow="2640" windowWidth="18010" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14710" yWindow="3410" windowWidth="18010" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Weekly</t>
   </si>
@@ -68,12 +68,6 @@
     <t>1, 3, 5, 10, 20, 50</t>
   </si>
   <si>
-    <t>k=1 of</t>
-  </si>
-  <si>
-    <t>k=50 of</t>
-  </si>
-  <si>
     <t>Worst case is all customers on one ledger with new PK per transaction</t>
   </si>
   <si>
@@ -189,6 +183,15 @@
   </si>
   <si>
     <t>Working on</t>
+  </si>
+  <si>
+    <t>k=1 best of</t>
+  </si>
+  <si>
+    <t>k=50 best of</t>
+  </si>
+  <si>
+    <t>Accuracy of a guess</t>
   </si>
 </sst>
 </file>
@@ -375,18 +378,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -394,22 +385,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -419,7 +405,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,31 +719,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="10" t="s">
+      <c r="A1" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="J1" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="H1" s="32"/>
+      <c r="J1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>9</v>
@@ -763,292 +766,340 @@
       <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="18">
         <f>(0.3982+0.3668+0.3843)/3</f>
         <v>0.3831</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="19">
         <f>(0.0224+0.0224+0.0237)/3</f>
         <v>2.2833333333333334E-2</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="18">
         <f>(0.5904+0.6326+0.5436)/3</f>
         <v>0.58886666666666665</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="19">
         <f>(0.0194+0.0194+0.0191)/3</f>
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="J3" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
+      <c r="G3" s="18">
+        <f>(0.7925)/1</f>
+        <v>0.79249999999999998</v>
+      </c>
+      <c r="H3" s="3">
+        <f>(0.0181)/1</f>
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="21">
         <f>(0.2535+0.2386+0.22)/3</f>
         <v>0.23736666666666664</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="22">
         <f>(0.1181+0.1143+0.1121)/3</f>
         <v>0.11483333333333334</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="21">
         <f>(0.3411+0.3014+0.3415)/3</f>
         <v>0.32800000000000001</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="22">
         <f>(0.1134+0.1125+0.1133)/3</f>
         <v>0.11306666666666666</v>
       </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
+      <c r="G4" s="23">
+        <f>(0.4382)/1</f>
+        <v>0.43819999999999998</v>
+      </c>
+      <c r="H4" s="24">
+        <f>(0.1034)/1</f>
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <f>(0.0884+0.0887+0.0886)/3</f>
         <v>8.8566666666666669E-2</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <f>(0.0158+0.0148+0.01523)/3</f>
         <v>1.5276666666666668E-2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="10">
         <f>(0.1263+0.1258+0.1273)/3</f>
         <v>0.12646666666666664</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>(0.02256+0.02296+0.02266)/3</f>
         <v>2.2726666666666669E-2</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="2">
+        <f>(0.1408)/1</f>
+        <v>0.14080000000000001</v>
+      </c>
+      <c r="H5" s="3">
+        <f>(0.0221)/1</f>
+        <v>2.2100000000000002E-2</v>
+      </c>
       <c r="J5" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="K5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="13"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="12">
         <f>(0.1218+0.1227+0.1243)/3</f>
         <v>0.12293333333333334</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="13">
         <f>(0.0903+0.0897+0.0904)/3</f>
         <v>9.0133333333333329E-2</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="12">
         <f>(0.1567+0.1565+0.1568)/3</f>
         <v>0.15666666666666668</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <f>(0.0924+0.0923+0.0921)/3</f>
         <v>9.2266666666666663E-2</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="4">
+        <f>(0.1756)/1</f>
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="H6" s="5">
+        <f>(0.0925)/1</f>
+        <v>9.2499999999999999E-2</v>
+      </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="30"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B8" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="26">
+        <f>1/300</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="26">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="35"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="36" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="18" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B23" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="18" t="s">
+      <c r="B24" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="18" t="s">
+      <c r="B25" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="18" t="s">
+      <c r="B26" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="J1:L2"/>
     <mergeCell ref="J3:L4"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Improved/clearer plan, updated KNN results after stripping 0s
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Semester1\Research\Smart-Grid-Blockchain-Privacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DF2BF2-132E-4F27-938F-2C1A3F6F3857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8808B49-EECE-4EEA-AEA5-FEB34A297B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14710" yWindow="3410" windowWidth="18010" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15410" yWindow="2200" windowWidth="18010" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Weekly</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Case</t>
   </si>
   <si>
-    <t>1, 3, 5, 10, 20, 50</t>
-  </si>
-  <si>
     <t>Worst case is all customers on one ledger with new PK per transaction</t>
   </si>
   <si>
@@ -92,30 +89,15 @@
     <t>1b</t>
   </si>
   <si>
-    <t>Classification accuracy of data points</t>
-  </si>
-  <si>
-    <t>Classification accuracy of data series</t>
-  </si>
-  <si>
     <t>Methods</t>
   </si>
   <si>
-    <t>MLP, KNN</t>
-  </si>
-  <si>
     <t>Variables</t>
   </si>
   <si>
     <t>Freq, ledgers, PKs</t>
   </si>
   <si>
-    <t>LTSM, Cointegration</t>
-  </si>
-  <si>
-    <t>Maybe clustering</t>
-  </si>
-  <si>
     <t>Stage 0</t>
   </si>
   <si>
@@ -125,21 +107,9 @@
     <t>2a</t>
   </si>
   <si>
-    <t>Include off-chain weather data: Source by postcode, find effective way to combine with Blockchain for analysis.</t>
-  </si>
-  <si>
     <t>2b</t>
   </si>
   <si>
-    <t>Adjusted version of 1a, same methods and variables for comparison. Changes needed to include extra data well.</t>
-  </si>
-  <si>
-    <t>2c</t>
-  </si>
-  <si>
-    <t>Refinements to techniques used in stage 1</t>
-  </si>
-  <si>
     <t>Stage 3</t>
   </si>
   <si>
@@ -176,29 +146,77 @@
     <t>Method</t>
   </si>
   <si>
-    <t>Currently running</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
     <t>Working on</t>
   </si>
   <si>
-    <t>k=1 best of</t>
-  </si>
-  <si>
-    <t>k=50 best of</t>
-  </si>
-  <si>
-    <t>Accuracy of a guess</t>
+    <t>Classification of sets of PKs</t>
+  </si>
+  <si>
+    <t>Plan to finish stage 1b</t>
+  </si>
+  <si>
+    <t>Guess accuracy</t>
+  </si>
+  <si>
+    <t>Classification of transactions</t>
+  </si>
+  <si>
+    <t>Features, LTSM, Cointegration</t>
+  </si>
+  <si>
+    <t>Add half hours</t>
+  </si>
+  <si>
+    <t>Add breakdown of accuracy</t>
+  </si>
+  <si>
+    <t>Confusion matrix, spread, standard dev etc</t>
+  </si>
+  <si>
+    <t>Reasons for methods</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>Stage 1a</t>
+  </si>
+  <si>
+    <t>Half Hourly</t>
+  </si>
+  <si>
+    <t>MLP, RF, KNN</t>
+  </si>
+  <si>
+    <t>Best of k=[1, 3, 5, 10, 20, 50]</t>
+  </si>
+  <si>
+    <t>Stage 2 measures the chance an attacker can find the customer's location from their dataset and solar data</t>
+  </si>
+  <si>
+    <t>Stage 1 establishes the likelihood to extract a user's dataset of transactions for stage 2</t>
+  </si>
+  <si>
+    <t>Explore whether solar data has an impact on stage 1 analysis.</t>
+  </si>
+  <si>
+    <t>Investigate approaches to combine a user data set with solar data to reveal postcode.</t>
+  </si>
+  <si>
+    <t>Stage 3 investigates methods to increase privacy and reduce the effectiveness of stage 1 and 2</t>
+  </si>
+  <si>
+    <t>Include off-chain weather data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +264,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +283,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,12 +376,23 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -347,37 +402,27 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -388,33 +433,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -423,8 +459,37 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -704,96 +769,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.81640625" customWidth="1"/>
     <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="8" width="9.453125" customWidth="1"/>
-    <col min="10" max="12" width="10" customWidth="1"/>
+    <col min="3" max="9" width="9.453125" customWidth="1"/>
+    <col min="11" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="31" t="s">
+    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="31" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="31" t="s">
+      <c r="F1" s="31"/>
+      <c r="G1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="J1" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="31"/>
+      <c r="K1" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+    </row>
+    <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+      <c r="I2" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="14">
         <f>(0.3982+0.3668+0.3843)/3</f>
         <v>0.3831</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="15">
         <f>(0.0224+0.0224+0.0237)/3</f>
         <v>2.2833333333333334E-2</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="14">
         <f>(0.5904+0.6326+0.5436)/3</f>
         <v>0.58886666666666665</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="15">
         <f>(0.0194+0.0194+0.0191)/3</f>
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="14">
         <f>(0.7925)/1</f>
         <v>0.79249999999999998</v>
       </c>
@@ -801,307 +876,423 @@
         <f>(0.0181)/1</f>
         <v>1.8100000000000002E-2</v>
       </c>
-      <c r="J3" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="34"/>
-      <c r="B4" s="20" t="s">
+      <c r="I3" s="40"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+    </row>
+    <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28"/>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="6">
         <f>(0.2535+0.2386+0.22)/3</f>
         <v>0.23736666666666664</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="7">
         <f>(0.1181+0.1143+0.1121)/3</f>
         <v>0.11483333333333334</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="6">
         <f>(0.3411+0.3014+0.3415)/3</f>
         <v>0.32800000000000001</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="7">
         <f>(0.1134+0.1125+0.1133)/3</f>
         <v>0.11306666666666666</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="2">
         <f>(0.4382)/1</f>
         <v>0.43819999999999998</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="3">
         <f>(0.1034)/1</f>
         <v>0.10340000000000001</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="40">
+        <f>(0.9811+0.9801+0.9793)/3</f>
+        <v>0.98016666666666652</v>
+      </c>
+      <c r="D5" s="15">
+        <f>(0.0042+0.0033+0.0035)/3</f>
+        <v>3.6666666666666666E-3</v>
+      </c>
+      <c r="E5" s="40">
+        <f>(1+1+1)/3</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <f>(0.0052+0.0049+0.0053)/3</f>
+        <v>5.1333333333333335E-3</v>
+      </c>
+      <c r="G5" s="40">
+        <f>(1+1+1)/3</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="41">
+        <f>(0.0068+0.007+0.0074)/3</f>
+        <v>7.0666666666666664E-3</v>
+      </c>
+      <c r="I5" s="40"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+    </row>
+    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="29"/>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8">
+        <f>(0.9797+0.9814+0.9793)/3</f>
+        <v>0.9801333333333333</v>
+      </c>
+      <c r="D6" s="9">
+        <f>(0.0044+0.0051+0.0047)/3</f>
+        <v>4.7333333333333333E-3</v>
+      </c>
+      <c r="E6" s="8">
+        <f>(1+1+1)/3</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="9">
+        <f>(0.0066+0.0064+0.0065)/3</f>
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="G6" s="8">
+        <f>(1+1+1)/3</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <f>(0.0079+0.0081+0.01)/3</f>
+        <v>8.666666666666668E-3</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10">
-        <f>(0.0884+0.0887+0.0886)/3</f>
-        <v>8.8566666666666669E-2</v>
-      </c>
-      <c r="D5" s="11">
-        <f>(0.0158+0.0148+0.01523)/3</f>
-        <v>1.5276666666666668E-2</v>
-      </c>
-      <c r="E5" s="10">
-        <f>(0.1263+0.1258+0.1273)/3</f>
-        <v>0.12646666666666664</v>
-      </c>
-      <c r="F5" s="11">
-        <f>(0.02256+0.02296+0.02266)/3</f>
-        <v>2.2726666666666669E-2</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="C7" s="6">
+        <f>(0.1062+0.1091+0.1051)/3</f>
+        <v>0.10680000000000001</v>
+      </c>
+      <c r="D7" s="7">
+        <f>(0.0214+0.02+0.0204)/3</f>
+        <v>2.06E-2</v>
+      </c>
+      <c r="E7" s="6">
+        <f>(0.1277+0.1276+0.1272)/3</f>
+        <v>0.12749999999999997</v>
+      </c>
+      <c r="F7" s="7">
+        <f>(0.0227+0.02273+0.0231)/3</f>
+        <v>2.284333333333333E-2</v>
+      </c>
+      <c r="G7" s="37">
         <f>(0.1408)/1</f>
         <v>0.14080000000000001</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H7" s="36">
         <f>(0.0221)/1</f>
         <v>2.2100000000000002E-2</v>
       </c>
-      <c r="J5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="36"/>
-      <c r="B6" s="6" t="s">
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+      <c r="K7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="29"/>
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12">
-        <f>(0.1218+0.1227+0.1243)/3</f>
-        <v>0.12293333333333334</v>
-      </c>
-      <c r="D6" s="13">
-        <f>(0.0903+0.0897+0.0904)/3</f>
-        <v>9.0133333333333329E-2</v>
-      </c>
-      <c r="E6" s="12">
-        <f>(0.1567+0.1565+0.1568)/3</f>
-        <v>0.15666666666666668</v>
-      </c>
-      <c r="F6" s="13">
-        <f>(0.0924+0.0923+0.0921)/3</f>
-        <v>9.2266666666666663E-2</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="C8" s="8">
+        <f>(0.1401+0.1378+0.1374)/3</f>
+        <v>0.13843333333333332</v>
+      </c>
+      <c r="D8" s="9">
+        <f>(0.1026+0.1017+0.1048)/3</f>
+        <v>0.10303333333333332</v>
+      </c>
+      <c r="E8" s="8">
+        <f>(0.1577+0.1582+0.1566)/3</f>
+        <v>0.1575</v>
+      </c>
+      <c r="F8" s="9">
+        <f>(0.0917+0.091+0.0914)/3</f>
+        <v>9.1366666666666665E-2</v>
+      </c>
+      <c r="G8" s="39">
         <f>(0.1756)/1</f>
         <v>0.17560000000000001</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H8" s="38">
         <f>(0.0925)/1</f>
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="J6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G7" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="30"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="27" t="s">
+      <c r="I8" s="8"/>
+      <c r="J8" s="9"/>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C10" s="17">
         <f>1/300</f>
         <v>3.3333333333333335E-3</v>
       </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="27" t="s">
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="21"/>
+      <c r="AB10" s="22"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C11" s="17">
         <f>1/100</f>
         <v>0.01</v>
       </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
+      <c r="B15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
+      <c r="B27" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>41</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A3:A4"/>
+  <mergeCells count="10">
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="K3:M4"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="J1:L2"/>
-    <mergeCell ref="J3:L4"/>
-    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F5:F6" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cointegration is a stage 2 thing now
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Semester1\Research\Smart-Grid-Blockchain-Privacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E0CC9A-D316-4B6B-B5EC-9364640FE3E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B3893-3F72-4615-B439-02DBA671286B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19650" yWindow="2450" windowWidth="18010" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15860" yWindow="3800" windowWidth="21490" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,13 +451,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,7 +463,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -757,7 +757,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,31 +769,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="43" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="43" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="43" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="44"/>
-      <c r="I1" s="43" t="s">
+      <c r="H1" s="42"/>
+      <c r="I1" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="39" t="s">
+      <c r="J1" s="42"/>
+      <c r="K1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
     </row>
     <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="23" t="s">
@@ -826,12 +826,12 @@
       <c r="J2" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -863,14 +863,14 @@
       </c>
       <c r="I3" s="33"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="45"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -900,12 +900,12 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="45" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -942,7 +942,7 @@
       <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="42"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="M6" s="19"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1014,7 +1014,7 @@
       </c>
     </row>
     <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="42"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Stage 1 raw results
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Semester1\Research\Smart-Grid-Blockchain-Privacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B3893-3F72-4615-B439-02DBA671286B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683CF6C3-1499-4231-8F2C-4056F0099253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="3800" windowWidth="21490" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15670" yWindow="3200" windowWidth="21490" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Weekly</t>
   </si>
@@ -134,27 +134,9 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Working on</t>
-  </si>
-  <si>
-    <t>Plan to finish stage 1b</t>
-  </si>
-  <si>
     <t>Guess accuracy</t>
   </si>
   <si>
-    <t>Add half hours</t>
-  </si>
-  <si>
-    <t>Add breakdown of accuracy</t>
-  </si>
-  <si>
-    <t>Confusion matrix, spread, standard dev etc</t>
-  </si>
-  <si>
-    <t>Reasons for methods</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -195,6 +177,9 @@
   </si>
   <si>
     <t>For identifying customer and postcode. On best and worst case scenarios.</t>
+  </si>
+  <si>
+    <t>Spread/STD DEV</t>
   </si>
 </sst>
 </file>
@@ -433,7 +418,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -472,6 +456,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -757,7 +742,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,31 +754,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="41" t="s">
+      <c r="A1" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="41" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="41" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="42"/>
-      <c r="K1" s="43" t="s">
+      <c r="H1" s="41"/>
+      <c r="I1" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="41"/>
+      <c r="K1" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="23" t="s">
@@ -802,36 +787,36 @@
       <c r="B2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -861,16 +846,16 @@
         <f>(0.0181)/1</f>
         <v>1.8100000000000002E-2</v>
       </c>
-      <c r="I3" s="33"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="39"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -900,18 +885,18 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
-        <v>40</v>
+      <c r="A5" s="44" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="32">
         <f>(0.9811+0.9801+0.9793)/3</f>
         <v>0.98016666666666652</v>
       </c>
@@ -919,7 +904,7 @@
         <f>(0.0042+0.0033+0.0035)/3</f>
         <v>3.6666666666666666E-3</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <f>(1+1+1)/3</f>
         <v>1</v>
       </c>
@@ -927,22 +912,22 @@
         <f>(0.0052+0.0049+0.0053)/3</f>
         <v>5.1333333333333335E-3</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="32">
         <f>(1+1+1)/3</f>
         <v>1</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="33">
         <f>(0.0068+0.007+0.0074)/3</f>
         <v>7.0666666666666664E-3</v>
       </c>
-      <c r="I5" s="33"/>
+      <c r="I5" s="32"/>
       <c r="J5" s="15"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
     </row>
     <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="40"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -977,7 +962,7 @@
       <c r="M6" s="19"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -999,22 +984,22 @@
         <f>(0.0227+0.02273+0.0231)/3</f>
         <v>2.284333333333333E-2</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="29">
         <f>(0.1408)/1</f>
         <v>0.14080000000000001</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="28">
         <f>(0.0221)/1</f>
         <v>2.2100000000000002E-2</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="40"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
@@ -1034,26 +1019,26 @@
         <f>(0.0917+0.091+0.0914)/3</f>
         <v>9.1366666666666665E-2</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <f>(0.1756)/1</f>
         <v>0.17560000000000001</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="30">
         <f>(0.0925)/1</f>
         <v>9.2499999999999999E-2</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
       <c r="K8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B10" s="18" t="s">
@@ -1064,14 +1049,12 @@
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="J10" s="21"/>
       <c r="AB10" s="22"/>
@@ -1085,27 +1068,21 @@
         <v>0.01</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="21"/>
+        <v>33</v>
+      </c>
+      <c r="G11" s="45"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="J12" s="21"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
@@ -1131,35 +1108,38 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
-      <c r="B16" s="38" t="s">
-        <v>45</v>
+      <c r="B16" s="37" t="s">
+        <v>39</v>
       </c>
       <c r="E16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
+      <c r="K16" s="20" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K17" s="20" t="s">
         <v>32</v>
       </c>
       <c r="M17" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="M18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
@@ -1167,13 +1147,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
-      <c r="B21" s="38" t="s">
-        <v>44</v>
+      <c r="B21" s="37" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
@@ -1181,7 +1161,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -1189,7 +1169,7 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
@@ -1205,8 +1185,8 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="10"/>
-      <c r="B26" s="38" t="s">
-        <v>48</v>
+      <c r="B26" s="37" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Half updated RF results, feature weight graphs, tuned RF depth
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Smart-Grid-Blockchain-Privacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726F9B88-93A1-4662-A86E-DB81A1176A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D289DCFD-3039-465E-B94F-C85953EEE7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9510" yWindow="7040" windowWidth="19180" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -954,7 +954,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1039,30 +1039,30 @@
         <v>0.23736666666666664</v>
       </c>
       <c r="D3" s="40">
-        <f>(0.1181+0.1143+0.1121)/3</f>
-        <v>0.11483333333333334</v>
+        <f>(0.0224+0.0224+0.0237)/3</f>
+        <v>2.2833333333333334E-2</v>
       </c>
       <c r="E3" s="18">
         <f>(0.3411+0.3014+0.3415)/3</f>
         <v>0.32800000000000001</v>
       </c>
       <c r="F3" s="8">
-        <f>(0.1134+0.1125+0.1133)/3</f>
-        <v>0.11306666666666666</v>
+        <f>(0.0194+0.0194+0.0191)/3</f>
+        <v>1.9300000000000001E-2</v>
       </c>
       <c r="G3" s="18">
         <f>(0.4382+0.471)/2</f>
         <v>0.4546</v>
       </c>
       <c r="H3" s="8">
-        <f>(0.1034+0.1005)/2</f>
-        <v>0.10195000000000001</v>
+        <f>(0.0181+0.0175)/2</f>
+        <v>1.7800000000000003E-2</v>
       </c>
       <c r="I3" s="40">
         <v>0.34549999999999997</v>
       </c>
       <c r="J3" s="8">
-        <v>9.8500000000000004E-2</v>
+        <v>1.95E-2</v>
       </c>
       <c r="K3" s="43" t="s">
         <v>10</v>
@@ -1080,30 +1080,30 @@
         <v>0.3831</v>
       </c>
       <c r="D4" s="41">
-        <f>(0.0224+0.0224+0.0237)/3</f>
-        <v>2.2833333333333334E-2</v>
+        <f>(0.1181+0.1143+0.1121)/3</f>
+        <v>0.11483333333333334</v>
       </c>
       <c r="E4" s="3">
         <f>(0.5904+0.6326+0.6324)/3</f>
         <v>0.61846666666666661</v>
       </c>
       <c r="F4" s="4">
-        <f>(0.0194+0.0194+0.0191)/3</f>
-        <v>1.9300000000000001E-2</v>
+        <f>(0.1134+0.1125+0.1133)/3</f>
+        <v>0.11306666666666666</v>
       </c>
       <c r="G4" s="3">
         <f>(0.7925+0.7477)/2</f>
         <v>0.77010000000000001</v>
       </c>
       <c r="H4" s="4">
-        <f>(0.0181+0.0175)/2</f>
-        <v>1.7800000000000003E-2</v>
+        <f>(0.1034+0.1005)/2</f>
+        <v>0.10195000000000001</v>
       </c>
       <c r="I4" s="41">
         <v>0.86660000000000004</v>
       </c>
       <c r="J4" s="4">
-        <v>1.95E-2</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="K4" s="43"/>
       <c r="L4" s="42"/>
@@ -1116,20 +1116,21 @@
       <c r="B5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="35">
-        <f>(0.9811+0.9801+0.9793)/3</f>
-        <v>0.98016666666666652</v>
-      </c>
-      <c r="D5" s="36">
-        <f>(0.0042+0.0033+0.0035)/3</f>
-        <v>3.6666666666666666E-3</v>
+      <c r="C5" s="18">
+        <f>(0.2991+0.251+0.3416)/3</f>
+        <v>0.29723333333333335</v>
+      </c>
+      <c r="D5" s="8">
+        <f>(0.0195+0.0203+0.02)/3</f>
+        <v>1.9933333333333334E-2</v>
       </c>
       <c r="E5" s="35">
-        <v>0.98750000000000004</v>
-      </c>
-      <c r="F5" s="36">
-        <f>(0.0052+0.0049+0.0053)/3</f>
-        <v>5.1333333333333335E-3</v>
+        <f>(0.2819+0.3097+0.3085)/3</f>
+        <v>0.30003333333333332</v>
+      </c>
+      <c r="F5" s="2">
+        <f>(0.0209+0.0207+0.0214)/3</f>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G5" s="35">
         <f>(1+1+1)/3</f>
@@ -1154,19 +1155,21 @@
       <c r="B6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="29">
-        <v>0.97870000000000001</v>
-      </c>
-      <c r="D6" s="30">
-        <f>(0.0044+0.0051+0.0047)/3</f>
-        <v>4.7333333333333333E-3</v>
+      <c r="C6" s="3">
+        <f>(0.2023+0.2018+0.2009)/3</f>
+        <v>0.20166666666666666</v>
+      </c>
+      <c r="D6" s="4">
+        <f>(0.1143+0.1132+0.1152)/3</f>
+        <v>0.11423333333333334</v>
       </c>
       <c r="E6" s="29">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="F6" s="30">
-        <f>(0.0066+0.0064+0.0065)/3</f>
-        <v>6.4999999999999997E-3</v>
+        <f>(0.1904+0.192+0.1887)/3</f>
+        <v>0.19036666666666668</v>
+      </c>
+      <c r="F6" s="4">
+        <f>(0.1134+0.1143+0.1151)/3</f>
+        <v>0.11426666666666667</v>
       </c>
       <c r="G6" s="29">
         <f>(1+1+1)/3</f>
@@ -1477,9 +1480,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="F5:F6" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed RF results completed
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Smart-Grid-Blockchain-Privacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B884E6A7-4366-423B-A6A4-999D330EC2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9740C2E1-6184-4059-9CF9-FE06622A7884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9510" yWindow="7040" windowWidth="19180" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6280" windowWidth="19180" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="114">
   <si>
     <t>Weekly</t>
   </si>
@@ -377,6 +377,9 @@
   <si>
     <t>Investigate classification methods: MLP, RF, KNN</t>
   </si>
+  <si>
+    <t>CNN</t>
+  </si>
 </sst>
 </file>
 
@@ -596,7 +599,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -623,6 +626,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,7 +654,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -641,34 +663,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -951,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -966,83 +972,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="41"/>
+      <c r="G1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="24" t="s">
+      <c r="H1" s="41"/>
+      <c r="I1" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="30">
         <f>(0.2535+0.2386+0.22)/3</f>
         <v>0.23736666666666664</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="28">
         <f>(0.0224+0.0224+0.0237)/3</f>
         <v>2.2833333333333334E-2</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="30">
         <f>(0.3411+0.3014+0.3415)/3</f>
         <v>0.32800000000000001</v>
       </c>
@@ -1050,7 +1056,7 @@
         <f>(0.0194+0.0194+0.0191)/3</f>
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="30">
         <f>(0.4382+0.471)/2</f>
         <v>0.4546</v>
       </c>
@@ -1058,32 +1064,32 @@
         <f>(0.0181+0.0175)/2</f>
         <v>1.7800000000000003E-2</v>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="33">
         <v>0.34549999999999997</v>
       </c>
       <c r="J3" s="8">
         <v>1.95E-2</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="22"/>
-      <c r="B4" s="29" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="31">
         <f>(0.3982+0.3668+0.3843)/3</f>
         <v>0.3831</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="29">
         <f>(0.1181+0.1143+0.1121)/3</f>
         <v>0.11483333333333334</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="31">
         <f>(0.5904+0.6326+0.6324)/3</f>
         <v>0.61846666666666661</v>
       </c>
@@ -1091,7 +1097,7 @@
         <f>(0.1134+0.1125+0.1133)/3</f>
         <v>0.11306666666666666</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="31">
         <f>(0.7925+0.7477)/2</f>
         <v>0.77010000000000001</v>
       </c>
@@ -1099,382 +1105,431 @@
         <f>(0.1034+0.1005)/2</f>
         <v>0.10195000000000001</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="34">
         <v>0.86660000000000004</v>
       </c>
       <c r="J4" s="4">
         <v>9.8500000000000004E-2</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28">
+        <f>(0.0844+0.0822+0.0857)/3</f>
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="D5" s="28">
+        <f>(0.0045+0.0045+0.0047)/3</f>
+        <v>4.5666666666666668E-3</v>
+      </c>
+      <c r="E5" s="46">
+        <f>(0.1172+0.1171+0.115)/3</f>
+        <v>0.11643333333333333</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="36"/>
+      <c r="B6" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="29">
+        <f>(0.1253+0.1224+0.1242)/3</f>
+        <v>0.12396666666666667</v>
+      </c>
+      <c r="D6" s="29">
+        <f>(0.106+0.1073+0.106)/3</f>
+        <v>0.10643333333333332</v>
+      </c>
+      <c r="E6" s="3">
+        <f>(0+0+0)/3</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A7" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C7" s="30">
         <f>(0.2023+0.2018+0.2009)/3</f>
         <v>0.20166666666666666</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D7" s="8">
         <f>(0.0195+0.0203+0.02)/3</f>
         <v>1.9933333333333334E-2</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E7" s="32">
         <f>(0.1904+0.192+0.1935)/3</f>
         <v>0.1919666666666667</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F7" s="2">
         <f>(0.0209+0.0207+0.0214)/3</f>
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G7" s="32">
         <f>(0.3159+0.3085+0)/3</f>
         <v>0.20813333333333336</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H7" s="2">
         <f>(0.0319+0.0309+0.031)/3</f>
         <v>3.1266666666666665E-2</v>
       </c>
-      <c r="I5" s="41">
-        <f>(0.1647+0.164+0)/3</f>
-        <v>0.10956666666666666</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="I7" s="32">
+        <f>(0.1647+0.164+0.1662)/3</f>
+        <v>0.16496666666666668</v>
+      </c>
+      <c r="J7" s="2">
         <f>(0.0209+0.0214+0.021)/3</f>
         <v>2.1099999999999997E-2</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-    </row>
-    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="23"/>
-      <c r="B6" s="34" t="s">
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="36"/>
+      <c r="B8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C8" s="31">
         <f>(0.2991+0.251+0.3416)/3</f>
         <v>0.29723333333333335</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D8" s="4">
         <f>(0.1143+0.1132+0.1152)/3</f>
         <v>0.11423333333333334</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E8" s="31">
         <f>(0.3082+0.3097+0.3085)/3</f>
         <v>0.30879999999999996</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F8" s="4">
         <f>(0.1134+0.1143+0.1151)/3</f>
         <v>0.11426666666666667</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G8" s="31">
         <f>(0.5418+0.5334+0)/3</f>
         <v>0.3584</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H8" s="4">
         <f>(0.1062+0.1066+0.1064)/3</f>
         <v>0.10639999999999999</v>
       </c>
-      <c r="I6" s="40">
-        <f>(0.2997+0.3176+0)/3</f>
-        <v>0.20576666666666665</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="I8" s="31">
+        <f>(0.2997+0.3176+0.3301)/3</f>
+        <v>0.31580000000000003</v>
+      </c>
+      <c r="J8" s="4">
         <f>(0.099+0.0987+0.0991)/3</f>
         <v>9.8933333333333318E-2</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B9" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C9" s="1">
         <f>(0.1062+0.1091+0.1051)/3</f>
         <v>0.10680000000000001</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D9" s="2">
         <f>(0.0097+0.0095+0.0093)/3</f>
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E9" s="1">
         <f>(0.1277+0.1276+0.1272)/3</f>
         <v>0.12749999999999997</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F9" s="2">
         <f>(0.0187+0.0184+0.0187)/3</f>
         <v>1.8600000000000002E-2</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G9" s="1">
         <f>(0.1408)/1</f>
         <v>0.14080000000000001</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H9" s="2">
         <f>(0.0221+0.0222)/2</f>
         <v>2.2150000000000003E-2</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I9" s="1">
         <v>8.5500000000000007E-2</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J9" s="2">
         <v>1.21E-2</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="23"/>
-      <c r="B8" s="34" t="s">
+    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="36"/>
+      <c r="B10" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C10" s="3">
         <f>(0.1401+0.1378+0.1374)/3</f>
         <v>0.13843333333333332</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D10" s="4">
         <f>(0.1026+0.1017+0.1048)/3</f>
         <v>0.10303333333333332</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E10" s="3">
         <f>(0.1577+0.1582+0.1566)/3</f>
         <v>0.1575</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F10" s="4">
         <f>(0.1071+0.1084+0.1071)/3</f>
         <v>0.10753333333333333</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G10" s="3">
         <f>(0.1756)/1</f>
         <v>0.17560000000000001</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H10" s="4">
         <f>(0.0925+0.0919)/2</f>
         <v>9.2200000000000004E-2</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I10" s="3">
         <v>0.1578</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J10" s="4">
         <v>8.3699999999999997E-2</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C12" s="10">
         <f>1/300</f>
         <v>3.3333333333333335E-3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="17"/>
-      <c r="AB10" s="14"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="B11" s="11" t="s">
+      <c r="E12" s="21"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="17"/>
+      <c r="AB12" s="14"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C13" s="10">
         <f>1/100</f>
         <v>0.01</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="17"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="G13" s="20"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="K16" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="5"/>
-      <c r="B17" t="s">
-        <v>112</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M17" t="s">
-        <v>43</v>
-      </c>
+      <c r="E17" s="6"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
+      <c r="B18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
       <c r="K18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="M18" t="s">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="5"/>
-      <c r="B21" s="19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+      <c r="B23" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
-      <c r="B26" s="19" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" t="s">
-        <v>29</v>
+        <v>20</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" t="s">
-        <v>29</v>
+      <c r="A28" s="5"/>
+      <c r="B28" s="19" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F50:F349">
-    <sortCondition ref="F50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F52:F351">
+    <sortCondition ref="F52"/>
   </sortState>
-  <mergeCells count="10">
-    <mergeCell ref="A7:A8"/>
+  <mergeCells count="11">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="K1:M2"/>
-    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>

<commit_message>
Improvements to CNN structure + weekly results
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EntireUniverse\UniStuff\2020\Smart-Grid-Blockchain-Privacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9740C2E1-6184-4059-9CF9-FE06622A7884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D849758-48F7-402B-8E84-C6BC265B5F35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="6280" windowWidth="19180" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,7 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,7 +599,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -640,11 +640,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -675,6 +670,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -960,7 +957,7 @@
   <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,31 +969,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="37" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="36"/>
+      <c r="G1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="37" t="s">
+      <c r="H1" s="36"/>
+      <c r="I1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="39" t="s">
+      <c r="J1" s="36"/>
+      <c r="K1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
@@ -1029,134 +1026,128 @@
       <c r="J2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:28" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="35" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="30">
-        <f>(0.2535+0.2386+0.22)/3</f>
-        <v>0.23736666666666664</v>
+      <c r="C3" s="41">
+        <f>(0.3982+0.3668+0.3843)/3</f>
+        <v>0.3831</v>
       </c>
       <c r="D3" s="28">
         <f>(0.0224+0.0224+0.0237)/3</f>
         <v>2.2833333333333334E-2</v>
       </c>
-      <c r="E3" s="30">
-        <f>(0.3411+0.3014+0.3415)/3</f>
-        <v>0.32800000000000001</v>
+      <c r="E3" s="41">
+        <f>(0.5904+0.6326+0.6324)/3</f>
+        <v>0.61846666666666661</v>
       </c>
       <c r="F3" s="8">
         <f>(0.0194+0.0194+0.0191)/3</f>
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="G3" s="30">
-        <f>(0.4382+0.471)/2</f>
-        <v>0.4546</v>
+      <c r="G3" s="41">
+        <f>(0.7925+0.7477)/2</f>
+        <v>0.77010000000000001</v>
       </c>
       <c r="H3" s="8">
         <f>(0.0181+0.0175)/2</f>
         <v>1.7800000000000003E-2</v>
       </c>
-      <c r="I3" s="33">
-        <v>0.34549999999999997</v>
+      <c r="I3" s="28">
+        <v>0.86660000000000004</v>
       </c>
       <c r="J3" s="8">
         <v>1.95E-2</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
     </row>
     <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="35"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="31">
-        <f>(0.3982+0.3668+0.3843)/3</f>
-        <v>0.3831</v>
+      <c r="C4" s="3">
+        <f>(0.2535+0.2386+0.22)/3</f>
+        <v>0.23736666666666664</v>
       </c>
       <c r="D4" s="29">
         <f>(0.1181+0.1143+0.1121)/3</f>
         <v>0.11483333333333334</v>
       </c>
-      <c r="E4" s="31">
-        <f>(0.5904+0.6326+0.6324)/3</f>
-        <v>0.61846666666666661</v>
+      <c r="E4" s="3">
+        <f>(0.3411+0.3014+0.3415)/3</f>
+        <v>0.32800000000000001</v>
       </c>
       <c r="F4" s="4">
         <f>(0.1134+0.1125+0.1133)/3</f>
         <v>0.11306666666666666</v>
       </c>
-      <c r="G4" s="31">
-        <f>(0.7925+0.7477)/2</f>
-        <v>0.77010000000000001</v>
+      <c r="G4" s="3">
+        <f>(0.4382+0.471)/2</f>
+        <v>0.4546</v>
       </c>
       <c r="H4" s="4">
         <f>(0.1034+0.1005)/2</f>
         <v>0.10195000000000001</v>
       </c>
-      <c r="I4" s="34">
-        <v>0.86660000000000004</v>
+      <c r="I4" s="29">
+        <v>0.34549999999999997</v>
       </c>
       <c r="J4" s="4">
         <v>9.8500000000000004E-2</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28">
-        <f>(0.0844+0.0822+0.0857)/3</f>
-        <v>8.4099999999999994E-2</v>
-      </c>
-      <c r="D5" s="28">
-        <f>(0.0045+0.0045+0.0047)/3</f>
-        <v>4.5666666666666668E-3</v>
-      </c>
-      <c r="E5" s="46">
-        <f>(0.1172+0.1171+0.115)/3</f>
-        <v>0.11643333333333333</v>
-      </c>
+      <c r="C5" s="42">
+        <f>(0.175+0.1714+0.1733)/3</f>
+        <v>0.17323333333333335</v>
+      </c>
+      <c r="D5" s="42">
+        <f>(0.0045+0.0044+0.0045)/3</f>
+        <v>4.4666666666666665E-3</v>
+      </c>
+      <c r="E5" s="41"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="46"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="46"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="36"/>
-      <c r="B6" s="45" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="29">
-        <f>(0.1253+0.1224+0.1242)/3</f>
-        <v>0.12396666666666667</v>
-      </c>
-      <c r="D6" s="29">
-        <f>(0.106+0.1073+0.106)/3</f>
-        <v>0.10643333333333332</v>
-      </c>
-      <c r="E6" s="3">
-        <f>(0+0+0)/3</f>
-        <v>0</v>
-      </c>
+      <c r="C6" s="43">
+        <f>(0.1536+0.158+0.1569)/3</f>
+        <v>0.15616666666666668</v>
+      </c>
+      <c r="D6" s="43">
+        <f>(0.1057+0.1054+0.1056)/3</f>
+        <v>0.10556666666666666</v>
+      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="4"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
@@ -1164,39 +1155,39 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="35" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="30">
-        <f>(0.2023+0.2018+0.2009)/3</f>
-        <v>0.20166666666666666</v>
+      <c r="C7" s="41">
+        <f>(0.2991+0.251+0.3416)/3</f>
+        <v>0.29723333333333335</v>
       </c>
       <c r="D7" s="8">
         <f>(0.0195+0.0203+0.02)/3</f>
         <v>1.9933333333333334E-2</v>
       </c>
-      <c r="E7" s="32">
-        <f>(0.1904+0.192+0.1935)/3</f>
-        <v>0.1919666666666667</v>
+      <c r="E7" s="1">
+        <f>(0.3082+0.3097+0.3085)/3</f>
+        <v>0.30879999999999996</v>
       </c>
       <c r="F7" s="2">
         <f>(0.0209+0.0207+0.0214)/3</f>
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G7" s="32">
-        <f>(0.3159+0.3085+0)/3</f>
-        <v>0.20813333333333336</v>
+      <c r="G7" s="1">
+        <f>(0.5418+0.5334+0)/3</f>
+        <v>0.3584</v>
       </c>
       <c r="H7" s="2">
         <f>(0.0319+0.0309+0.031)/3</f>
         <v>3.1266666666666665E-2</v>
       </c>
-      <c r="I7" s="32">
-        <f>(0.1647+0.164+0.1662)/3</f>
-        <v>0.16496666666666668</v>
+      <c r="I7" s="1">
+        <f>(0.2997+0.3176+0.3301)/3</f>
+        <v>0.31580000000000003</v>
       </c>
       <c r="J7" s="2">
         <f>(0.0209+0.0214+0.021)/3</f>
@@ -1207,37 +1198,37 @@
       <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="36"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="31">
-        <f>(0.2991+0.251+0.3416)/3</f>
-        <v>0.29723333333333335</v>
+      <c r="C8" s="3">
+        <f>(0.2023+0.2018+0.2009)/3</f>
+        <v>0.20166666666666666</v>
       </c>
       <c r="D8" s="4">
         <f>(0.1143+0.1132+0.1152)/3</f>
         <v>0.11423333333333334</v>
       </c>
-      <c r="E8" s="31">
-        <f>(0.3082+0.3097+0.3085)/3</f>
-        <v>0.30879999999999996</v>
+      <c r="E8" s="3">
+        <f>(0.1904+0.192+0.1935)/3</f>
+        <v>0.1919666666666667</v>
       </c>
       <c r="F8" s="4">
         <f>(0.1134+0.1143+0.1151)/3</f>
         <v>0.11426666666666667</v>
       </c>
-      <c r="G8" s="31">
-        <f>(0.5418+0.5334+0)/3</f>
-        <v>0.3584</v>
+      <c r="G8" s="3">
+        <f>(0.3159+0.3085+0)/3</f>
+        <v>0.20813333333333336</v>
       </c>
       <c r="H8" s="4">
         <f>(0.1062+0.1066+0.1064)/3</f>
         <v>0.10639999999999999</v>
       </c>
-      <c r="I8" s="31">
-        <f>(0.2997+0.3176+0.3301)/3</f>
-        <v>0.31580000000000003</v>
+      <c r="I8" s="3">
+        <f>(0.1647+0.164+0.1662)/3</f>
+        <v>0.16496666666666668</v>
       </c>
       <c r="J8" s="4">
         <f>(0.099+0.0987+0.0991)/3</f>
@@ -1248,10 +1239,10 @@
       <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="39" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1">
@@ -1289,8 +1280,8 @@
       </c>
     </row>
     <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="36"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3">

</xml_diff>

<commit_message>
Updated results and graphs
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="116">
   <si>
     <t xml:space="preserve">Stage 1a</t>
   </si>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">CNN</t>
   </si>
   <si>
-    <t xml:space="preserve">RDF</t>
+    <t xml:space="preserve">RFC</t>
   </si>
   <si>
     <t xml:space="preserve">KNN</t>
@@ -99,7 +99,7 @@
     <t xml:space="preserve">Stage 1 establishes the likelihood to extract a user's dataset of transactions for stage 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Investigate classification methods: MLP, CNN, RF, KNN</t>
+    <t xml:space="preserve">Investigate classification methods: MLP, CNN, RFC, KNN</t>
   </si>
   <si>
     <t xml:space="preserve">What's the likelihood one can see a transaction and pick the customer or postcode?</t>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve">Worst case is all customers on one ledger with new PK per transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDF</t>
   </si>
   <si>
     <t xml:space="preserve">Investigate classification methods: MLP, RF, KNN</t>
@@ -438,7 +441,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,31 +451,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
-        <bgColor rgb="FFE2F0D9"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
-        <bgColor rgb="FFDAE3F3"/>
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF92D050"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF70AD47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF70AD47"/>
-        <bgColor rgb="FF92D050"/>
+        <bgColor rgb="FF81D41A"/>
       </patternFill>
     </fill>
     <fill>
@@ -588,7 +585,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -625,7 +622,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,10 +631,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -669,11 +662,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -689,10 +686,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -701,8 +694,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -741,8 +734,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -757,7 +754,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -777,6 +774,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,19 +790,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -830,7 +831,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF92D050"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -850,7 +851,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFE2F0D9"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -884,8 +885,8 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -978,126 +979,126 @@
         <v>11</v>
       </c>
       <c r="C3" s="11" t="n">
-        <f aca="false">(0.4804+0.4479+0.4332)/3</f>
-        <v>0.453833333333333</v>
+        <f aca="false">(0.4604+0.4579+0.4532)/3</f>
+        <v>0.457166666666667</v>
       </c>
       <c r="D3" s="12" t="n">
-        <f aca="false">(0.4581+0.4505+0.4579)/3</f>
-        <v>0.4555</v>
-      </c>
-      <c r="E3" s="13" t="n">
+        <f aca="false">(0.4781+0.4705+0.4879)/3</f>
+        <v>0.478833333333333</v>
+      </c>
+      <c r="E3" s="12" t="n">
         <f aca="false">(0.0224+0.0224+0.0237)/3</f>
         <v>0.0228333333333333</v>
       </c>
       <c r="F3" s="11" t="n">
-        <f aca="false">(0.7251+0.649+0.6612)/3</f>
-        <v>0.678433333333333</v>
+        <f aca="false">(0.6451+0.649+0.6312)/3</f>
+        <v>0.641766666666667</v>
       </c>
       <c r="G3" s="12" t="n">
-        <f aca="false">(0.5581+0.6302+0.6051)/3</f>
-        <v>0.5978</v>
-      </c>
-      <c r="H3" s="14" t="n">
+        <f aca="false">(0.6481+0.6702+0.6651)/3</f>
+        <v>0.661133333333333</v>
+      </c>
+      <c r="H3" s="13" t="n">
         <f aca="false">(0.0194+0.0194+0.0191)/3</f>
         <v>0.0193</v>
       </c>
       <c r="I3" s="11" t="n">
-        <f aca="false">(0.7046+0.7305)/2</f>
-        <v>0.71755</v>
+        <f aca="false">(0.7546+0.7505)/2</f>
+        <v>0.75255</v>
       </c>
       <c r="J3" s="12" t="n">
-        <f aca="false">(0.8658+0.6147)/2</f>
-        <v>0.74025</v>
-      </c>
-      <c r="K3" s="14" t="n">
-        <f aca="false">(0.0181+0.0175)/2</f>
-        <v>0.0178</v>
+        <f aca="false">(0.7658+0.7747)/2</f>
+        <v>0.77025</v>
+      </c>
+      <c r="K3" s="13" t="n">
+        <f aca="false">(0.0181+0.0185)/2</f>
+        <v>0.0183</v>
       </c>
       <c r="L3" s="11" t="n">
-        <f aca="false">(0.8586+0.8659)/2</f>
-        <v>0.86225</v>
+        <f aca="false">(0.7386+0.7359)/2</f>
+        <v>0.73725</v>
       </c>
       <c r="M3" s="12" t="n">
-        <f aca="false">(0.7814+0.8305)/2</f>
-        <v>0.80595</v>
-      </c>
-      <c r="N3" s="14" t="n">
-        <f aca="false">(0.0195+0.0186)/2</f>
-        <v>0.01905</v>
+        <f aca="false">(0.7614+0.7605)/2</f>
+        <v>0.76095</v>
+      </c>
+      <c r="N3" s="13" t="n">
+        <f aca="false">(0.0185+0.0186)/2</f>
+        <v>0.01855</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16" t="n">
-        <f aca="false">(0.2311+0.2235+0.231)/3</f>
-        <v>0.228533333333333</v>
-      </c>
-      <c r="D4" s="17" t="n">
+      <c r="C4" s="15" t="n">
+        <f aca="false">(0.2211+0.2235+0.231)/3</f>
+        <v>0.2252</v>
+      </c>
+      <c r="D4" s="16" t="n">
         <f aca="false">(0.2656+0.2412+0.2432)/3</f>
         <v>0.25</v>
       </c>
-      <c r="E4" s="17" t="n">
+      <c r="E4" s="16" t="n">
         <f aca="false">(0.1181+0.1143+0.1121)/3</f>
         <v>0.114833333333333</v>
       </c>
-      <c r="F4" s="16" t="n">
-        <f aca="false">(0.3197+0.3895+0.3044)/3</f>
-        <v>0.337866666666667</v>
-      </c>
-      <c r="G4" s="17" t="n">
+      <c r="F4" s="15" t="n">
+        <f aca="false">(0.3197+0.3195+0.3044)/3</f>
+        <v>0.314533333333333</v>
+      </c>
+      <c r="G4" s="16" t="n">
         <f aca="false">(0.3627+0.311+0.3503)/3</f>
         <v>0.341333333333333</v>
       </c>
-      <c r="H4" s="18" t="n">
+      <c r="H4" s="17" t="n">
         <f aca="false">(0.1134+0.1125+0.1133)/3</f>
         <v>0.113066666666667</v>
       </c>
-      <c r="I4" s="16" t="n">
-        <f aca="false">(0.4742+0.4024)/2</f>
-        <v>0.4383</v>
-      </c>
-      <c r="J4" s="17" t="n">
-        <f aca="false">(0.3341+0.2801)/2</f>
-        <v>0.3071</v>
-      </c>
-      <c r="K4" s="18" t="n">
+      <c r="I4" s="15" t="n">
+        <f aca="false">(0.4042+0.4024)/2</f>
+        <v>0.4033</v>
+      </c>
+      <c r="J4" s="16" t="n">
+        <f aca="false">(0.4341+0.4301)/2</f>
+        <v>0.4321</v>
+      </c>
+      <c r="K4" s="17" t="n">
         <f aca="false">(0.1034+0.1005)/2</f>
         <v>0.10195</v>
       </c>
-      <c r="L4" s="16" t="n">
-        <f aca="false">(0.3692+0.4044)/2</f>
-        <v>0.3868</v>
-      </c>
-      <c r="M4" s="17" t="n">
-        <f aca="false">(0.3057+0.3882)/2</f>
-        <v>0.34695</v>
-      </c>
-      <c r="N4" s="18" t="n">
+      <c r="L4" s="15" t="n">
+        <f aca="false">(0.3692+0.3644)/2</f>
+        <v>0.3668</v>
+      </c>
+      <c r="M4" s="16" t="n">
+        <f aca="false">(0.3857+0.3882)/2</f>
+        <v>0.38695</v>
+      </c>
+      <c r="N4" s="17" t="n">
         <f aca="false">(0.0985+0.0986)/2</f>
         <v>0.09855</v>
       </c>
-      <c r="O4" s="19"/>
+      <c r="O4" s="18"/>
       <c r="P4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12" t="n">
+      <c r="C5" s="21" t="n">
         <f aca="false">(0.5701+0.5895+0.5812)/3</f>
         <v>0.580266666666667</v>
       </c>
-      <c r="D5" s="13" t="n">
-        <f aca="false">(0.5804+0.5966+0.5493)/3</f>
-        <v>0.575433333333333</v>
-      </c>
-      <c r="E5" s="13" t="n">
+      <c r="D5" s="12" t="n">
+        <f aca="false">(0.5804+0.5966+0.5993)/3</f>
+        <v>0.5921</v>
+      </c>
+      <c r="E5" s="12" t="n">
         <f aca="false">(0.026+0.0242+0.0238)/3</f>
         <v>0.0246666666666667</v>
       </c>
@@ -1106,10 +1107,10 @@
         <v>0.6991</v>
       </c>
       <c r="G5" s="23" t="n">
-        <f aca="false">(0.7+0.7115+0.7099)/3</f>
-        <v>0.707133333333333</v>
-      </c>
-      <c r="H5" s="14" t="n">
+        <f aca="false">(0.71+0.7115+0.7099)/3</f>
+        <v>0.710466666666667</v>
+      </c>
+      <c r="H5" s="13" t="n">
         <f aca="false">(0.0238+0.0237+0.0242)/3</f>
         <v>0.0239</v>
       </c>
@@ -1118,82 +1119,82 @@
         <v>0.78915</v>
       </c>
       <c r="J5" s="23" t="n">
-        <f aca="false">(0.7934+0.7845)/2</f>
-        <v>0.78895</v>
-      </c>
-      <c r="K5" s="14" t="n">
+        <f aca="false">(0.7934+0.7945)/2</f>
+        <v>0.79395</v>
+      </c>
+      <c r="K5" s="13" t="n">
         <f aca="false">(0.0234+0.0232)/2</f>
         <v>0.0233</v>
       </c>
-      <c r="L5" s="25" t="n">
-        <f aca="false">(0.7906+0.7889)/2</f>
-        <v>0.78975</v>
+      <c r="L5" s="24" t="n">
+        <f aca="false">(0.8406+0.8389)/2</f>
+        <v>0.83975</v>
       </c>
       <c r="M5" s="23" t="n">
-        <f aca="false">(0.8045+0.7897)/2</f>
-        <v>0.7971</v>
-      </c>
-      <c r="N5" s="14" t="n">
+        <f aca="false">(0.8445+0.8597)/2</f>
+        <v>0.8521</v>
+      </c>
+      <c r="N5" s="13" t="n">
         <f aca="false">(0.0252+0.0244)/2</f>
         <v>0.0248</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20"/>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="17" t="n">
+      <c r="C6" s="16" t="n">
         <f aca="false">(0.429+0.4242+0.4323)/3</f>
         <v>0.4285</v>
       </c>
-      <c r="D6" s="27" t="n">
-        <f aca="false">(0.4515+0.4418+0.4561)/3</f>
-        <v>0.4498</v>
-      </c>
-      <c r="E6" s="17" t="n">
+      <c r="D6" s="26" t="n">
+        <f aca="false">(0.4515+0.4618+0.4561)/3</f>
+        <v>0.456466666666667</v>
+      </c>
+      <c r="E6" s="16" t="n">
         <f aca="false">(0.1169+0.1121+0.1149)/3</f>
         <v>0.114633333333333</v>
       </c>
-      <c r="F6" s="16" t="n">
+      <c r="F6" s="15" t="n">
         <f aca="false">(0.5249+0.5418+0.5522)/3</f>
         <v>0.539633333333333</v>
       </c>
-      <c r="G6" s="27" t="n">
-        <f aca="false">(0.5438+0.5666+0.5428)/3</f>
-        <v>0.551066666666667</v>
-      </c>
-      <c r="H6" s="18" t="n">
+      <c r="G6" s="26" t="n">
+        <f aca="false">(0.5538+0.5666+0.5528)/3</f>
+        <v>0.557733333333333</v>
+      </c>
+      <c r="H6" s="17" t="n">
         <f aca="false">(0.1146+0.1146+0.115)/3</f>
         <v>0.114733333333333</v>
       </c>
-      <c r="I6" s="16" t="n">
+      <c r="I6" s="15" t="n">
         <f aca="false">(0.6052+0.6316)/2</f>
         <v>0.6184</v>
       </c>
-      <c r="J6" s="27" t="n">
-        <f aca="false">(0.6067+0.629)/2</f>
-        <v>0.61785</v>
-      </c>
-      <c r="K6" s="18" t="n">
+      <c r="J6" s="26" t="n">
+        <f aca="false">(0.6267+0.629)/2</f>
+        <v>0.62785</v>
+      </c>
+      <c r="K6" s="17" t="n">
         <f aca="false">(0.1011+0.1012)/2</f>
         <v>0.10115</v>
       </c>
-      <c r="L6" s="16" t="n">
+      <c r="L6" s="15" t="n">
         <f aca="false">(0.6182+0.6173)/2</f>
         <v>0.61775</v>
       </c>
-      <c r="M6" s="17" t="n">
-        <f aca="false">(0.6306+0.6182)/2</f>
-        <v>0.6244</v>
-      </c>
-      <c r="N6" s="18" t="n">
+      <c r="M6" s="26" t="n">
+        <f aca="false">(0.6306+0.6382)/2</f>
+        <v>0.6344</v>
+      </c>
+      <c r="N6" s="17" t="n">
         <f aca="false">(0.0999+0.1007)/2</f>
         <v>0.1003</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1203,15 +1204,15 @@
         <f aca="false">(0.4325+0.4169+0.4658)/3</f>
         <v>0.4384</v>
       </c>
-      <c r="D7" s="13" t="n">
-        <f aca="false">(0.4204+0.448+0.4105)/3</f>
-        <v>0.4263</v>
-      </c>
-      <c r="E7" s="14" t="n">
+      <c r="D7" s="12" t="n">
+        <f aca="false">(0.4404+0.448+0.4405)/3</f>
+        <v>0.442966666666667</v>
+      </c>
+      <c r="E7" s="13" t="n">
         <f aca="false">(0.0195+0.0203+0.02)/3</f>
         <v>0.0199333333333333</v>
       </c>
-      <c r="F7" s="25" t="n">
+      <c r="F7" s="27" t="n">
         <f aca="false">(0.4323+0.3849+0.3826)/3</f>
         <v>0.399933333333333</v>
       </c>
@@ -1219,31 +1220,31 @@
         <f aca="false">(0.4254+0.4457+0.4062)/3</f>
         <v>0.425766666666667</v>
       </c>
-      <c r="H7" s="29" t="n">
+      <c r="H7" s="28" t="n">
         <f aca="false">(0.0209+0.0207+0.0214)/3</f>
         <v>0.021</v>
       </c>
-      <c r="I7" s="25" t="n">
-        <f aca="false">(0.3599+0.3914)/2</f>
-        <v>0.37565</v>
+      <c r="I7" s="27" t="n">
+        <f aca="false">(0.3599+0.3714)/2</f>
+        <v>0.36565</v>
       </c>
       <c r="J7" s="23" t="n">
-        <f aca="false">(0.3398+0.3561)/2</f>
-        <v>0.34795</v>
-      </c>
-      <c r="K7" s="29" t="n">
-        <f aca="false">(0.0309+0.031)/3</f>
-        <v>0.0206333333333333</v>
-      </c>
-      <c r="L7" s="25" t="n">
+        <f aca="false">(0.3698+0.3561)/2</f>
+        <v>0.36295</v>
+      </c>
+      <c r="K7" s="28" t="n">
+        <f aca="false">(0.0259+0.025)/2</f>
+        <v>0.02545</v>
+      </c>
+      <c r="L7" s="27" t="n">
         <f aca="false">(0.3481+0.3196)/2</f>
         <v>0.33385</v>
       </c>
       <c r="M7" s="23" t="n">
-        <f aca="false">(0.3744+0.3257)/2</f>
-        <v>0.35005</v>
-      </c>
-      <c r="N7" s="29" t="n">
+        <f aca="false">(0.3444+0.3257)/2</f>
+        <v>0.33505</v>
+      </c>
+      <c r="N7" s="28" t="n">
         <f aca="false">(0.0209+0.0214)/2</f>
         <v>0.02115</v>
       </c>
@@ -1252,55 +1253,55 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28"/>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="16" t="n">
+      <c r="C8" s="15" t="n">
         <f aca="false">(0.2376+0.2338+0.235)/3</f>
         <v>0.235466666666667</v>
       </c>
-      <c r="D8" s="17" t="n">
+      <c r="D8" s="16" t="n">
         <f aca="false">(0.2633+0.2577+0.2631)/3</f>
         <v>0.261366666666667</v>
       </c>
-      <c r="E8" s="18" t="n">
+      <c r="E8" s="17" t="n">
         <f aca="false">(0.1143+0.1132+0.1152)/3</f>
         <v>0.114233333333333</v>
       </c>
-      <c r="F8" s="16" t="n">
+      <c r="F8" s="15" t="n">
         <f aca="false">(0.265+0.2708+0.2727)/3</f>
         <v>0.2695</v>
       </c>
-      <c r="G8" s="17" t="n">
-        <f aca="false">(0.2735+0.2645+0.2689)/3</f>
-        <v>0.268966666666667</v>
-      </c>
-      <c r="H8" s="18" t="n">
+      <c r="G8" s="16" t="n">
+        <f aca="false">(0.2735+0.2845+0.2889)/3</f>
+        <v>0.2823</v>
+      </c>
+      <c r="H8" s="17" t="n">
         <f aca="false">(0.1134+0.1143+0.1151)/3</f>
         <v>0.114266666666667</v>
       </c>
-      <c r="I8" s="16" t="n">
+      <c r="I8" s="15" t="n">
         <f aca="false">(0.232+0.2333)/2</f>
         <v>0.23265</v>
       </c>
-      <c r="J8" s="17" t="n">
+      <c r="J8" s="16" t="n">
         <f aca="false">(0.2377+0.2336)/2</f>
         <v>0.23565</v>
       </c>
-      <c r="K8" s="18" t="n">
-        <f aca="false">(0.1066+0.1064)/3</f>
-        <v>0.071</v>
-      </c>
-      <c r="L8" s="16" t="n">
+      <c r="K8" s="17" t="n">
+        <f aca="false">(0.1066+0.1064)/2</f>
+        <v>0.1065</v>
+      </c>
+      <c r="L8" s="15" t="n">
         <f aca="false">(0.2254+0.2285)/2</f>
         <v>0.22695</v>
       </c>
-      <c r="M8" s="17" t="n">
+      <c r="M8" s="16" t="n">
         <f aca="false">(0.2164+0.292)/2</f>
         <v>0.2542</v>
       </c>
-      <c r="N8" s="18" t="n">
+      <c r="N8" s="17" t="n">
         <f aca="false">(0.099+0.0987)/2</f>
         <v>0.09885</v>
       </c>
@@ -1309,13 +1310,13 @@
       <c r="Q8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="25" t="n">
+      <c r="C9" s="27" t="n">
         <f aca="false">(0.3587+0.3632+0.3573)/3</f>
         <v>0.359733333333333</v>
       </c>
@@ -1323,11 +1324,11 @@
         <f aca="false">(0.3498+0.3479+0.3496)/3</f>
         <v>0.3491</v>
       </c>
-      <c r="E9" s="29" t="n">
+      <c r="E9" s="28" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
-      <c r="F9" s="25" t="n">
+      <c r="F9" s="27" t="n">
         <f aca="false">(0.4789+0.4773+0.4784)/3</f>
         <v>0.4782</v>
       </c>
@@ -1335,11 +1336,11 @@
         <f aca="false">(0.4779+0.4776+0.4793)/3</f>
         <v>0.478266666666667</v>
       </c>
-      <c r="H9" s="29" t="n">
+      <c r="H9" s="28" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
-      <c r="I9" s="25" t="n">
+      <c r="I9" s="27" t="n">
         <f aca="false">(0.5451+0.5452)/2</f>
         <v>0.54515</v>
       </c>
@@ -1347,19 +1348,19 @@
         <f aca="false">(0.5451+0.5456)/2</f>
         <v>0.54535</v>
       </c>
-      <c r="K9" s="29" t="n">
+      <c r="K9" s="28" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
-      <c r="L9" s="25" t="n">
-        <f aca="false">(0.5542+0.5538)/2</f>
-        <v>0.554</v>
+      <c r="L9" s="27" t="n">
+        <f aca="false">(0.5042+0.508)/2</f>
+        <v>0.5061</v>
       </c>
       <c r="M9" s="23" t="n">
-        <f aca="false">(0.5545+0.5546)/2</f>
-        <v>0.55455</v>
-      </c>
-      <c r="N9" s="29" t="n">
+        <f aca="false">(0.5145+0.5146)/2</f>
+        <v>0.51455</v>
+      </c>
+      <c r="N9" s="28" t="n">
         <f aca="false">(0.0239+0.0239)/2</f>
         <v>0.0239</v>
       </c>
@@ -1368,55 +1369,55 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="16" t="n">
+      <c r="C10" s="15" t="n">
         <f aca="false">(0.2334+0.2216+0.2369)/3</f>
         <v>0.230633333333333</v>
       </c>
-      <c r="D10" s="17" t="n">
+      <c r="D10" s="16" t="n">
         <f aca="false">(0.2643+0.2638+0.2651)/3</f>
         <v>0.2644</v>
       </c>
-      <c r="E10" s="18" t="n">
-        <f aca="false">(0.1026+0.1017+0.1048)/3</f>
-        <v>0.103033333333333</v>
-      </c>
-      <c r="F10" s="16" t="n">
+      <c r="E10" s="17" t="n">
+        <f aca="false">(0.1046+0.1047+0.1048)/3</f>
+        <v>0.1047</v>
+      </c>
+      <c r="F10" s="15" t="n">
         <f aca="false">(0.3778+0.3786+0.3819)/3</f>
         <v>0.379433333333333</v>
       </c>
-      <c r="G10" s="17" t="n">
+      <c r="G10" s="16" t="n">
         <f aca="false">(0.3804+0.3778+0.3795)/3</f>
         <v>0.379233333333333</v>
       </c>
-      <c r="H10" s="18" t="n">
-        <f aca="false">(0.1071+0.1084+0.1071)/3</f>
-        <v>0.107533333333333</v>
-      </c>
-      <c r="I10" s="16" t="n">
+      <c r="H10" s="17" t="n">
+        <f aca="false">(0.1071+0.1064+0.1071)/3</f>
+        <v>0.106866666666667</v>
+      </c>
+      <c r="I10" s="15" t="n">
         <f aca="false">(0.4336+0.4341)/2</f>
         <v>0.43385</v>
       </c>
-      <c r="J10" s="17" t="n">
+      <c r="J10" s="16" t="n">
         <f aca="false">(0.4346+0.4346)/2</f>
         <v>0.4346</v>
       </c>
-      <c r="K10" s="18" t="n">
-        <f aca="false">(0.0925+0.0919)/2</f>
-        <v>0.0922</v>
-      </c>
-      <c r="L10" s="16" t="n">
-        <f aca="false">(0.4355+0.4357)/2</f>
-        <v>0.4356</v>
-      </c>
-      <c r="M10" s="17" t="n">
-        <f aca="false">(0.4357+0.4357)/2</f>
-        <v>0.4357</v>
-      </c>
-      <c r="N10" s="18" t="n">
+      <c r="K10" s="17" t="n">
+        <f aca="false">(0.0975+0.0979)/2</f>
+        <v>0.0977</v>
+      </c>
+      <c r="L10" s="15" t="n">
+        <f aca="false">(0.3855+0.3857)/2</f>
+        <v>0.3856</v>
+      </c>
+      <c r="M10" s="16" t="n">
+        <f aca="false">(0.3957+0.3957)/2</f>
+        <v>0.3957</v>
+      </c>
+      <c r="N10" s="17" t="n">
         <f aca="false">(0.0952+0.0952)/2</f>
         <v>0.0952</v>
       </c>
@@ -1425,63 +1426,63 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="35"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="34"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="38" t="s">
+      <c r="O13" s="37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="O16" s="38" t="s">
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="O16" s="37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="38" t="s">
+      <c r="O17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="Q17" s="0" t="s">
@@ -1489,11 +1490,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="38" t="s">
+      <c r="O18" s="37" t="s">
         <v>20</v>
       </c>
       <c r="Q18" s="0" t="s">
@@ -1501,21 +1502,21 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="36" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36"/>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="34" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="35" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -1523,7 +1524,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="35" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -1531,27 +1532,27 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36"/>
+      <c r="A24" s="35"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36"/>
-      <c r="B26" s="35" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="0" t="s">
@@ -1559,10 +1560,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="33" t="s">
         <v>42</v>
       </c>
       <c r="H28" s="0" t="s">
@@ -1570,18 +1571,18 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="33" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1614,7 +1615,7 @@
   </sheetPr>
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1705,7 +1706,7 @@
       <c r="Q2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="38" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1759,8 +1760,8 @@
       <c r="Q3" s="43"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="38"/>
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="44" t="n">
@@ -1810,10 +1811,10 @@
       <c r="Q4" s="43"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="40" t="n">
@@ -1860,8 +1861,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="28"/>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="45" t="n">
@@ -1908,8 +1909,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28" t="s">
-        <v>14</v>
+      <c r="A7" s="47" t="s">
+        <v>49</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
@@ -1926,33 +1927,33 @@
         <f aca="false">(0.0195+0.0203+0.02)/3</f>
         <v>0.0199333333333333</v>
       </c>
-      <c r="F7" s="47" t="n">
+      <c r="F7" s="48" t="n">
         <f aca="false">(0.3343+0.3376+0.3375)/3</f>
         <v>0.336466666666667</v>
       </c>
-      <c r="G7" s="48" t="n">
+      <c r="G7" s="49" t="n">
         <f aca="false">(0.2274+0.2273+0.2291)/3</f>
         <v>0.227933333333333</v>
       </c>
-      <c r="H7" s="49" t="n">
+      <c r="H7" s="50" t="n">
         <f aca="false">(0.0209+0.0207+0.0214)/3</f>
         <v>0.021</v>
       </c>
-      <c r="I7" s="47" t="n">
+      <c r="I7" s="48" t="n">
         <f aca="false">(0.3418+0.3334+0.3179)/3</f>
         <v>0.331033333333333</v>
       </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49" t="n">
+      <c r="J7" s="49"/>
+      <c r="K7" s="50" t="n">
         <f aca="false">(0.0319+0.0309+0.031)/3</f>
         <v>0.0312666666666667</v>
       </c>
-      <c r="L7" s="47" t="n">
+      <c r="L7" s="48" t="n">
         <f aca="false">(0.2997+0.3176+0.3301)/3</f>
         <v>0.3158</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="49" t="n">
+      <c r="M7" s="49"/>
+      <c r="N7" s="50" t="n">
         <f aca="false">(0.0209+0.0214)/2</f>
         <v>0.02115</v>
       </c>
@@ -1961,8 +1962,8 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28"/>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="47"/>
+      <c r="B8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="44" t="n">
@@ -2012,50 +2013,50 @@
       <c r="Q8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="47" t="n">
+      <c r="C9" s="48" t="n">
         <f aca="false">(0.1062+0.1091+0.1051)/3</f>
         <v>0.1068</v>
       </c>
-      <c r="D9" s="48" t="n">
+      <c r="D9" s="49" t="n">
         <f aca="false">(0.085+0.0874+0.0856)/3</f>
         <v>0.086</v>
       </c>
-      <c r="E9" s="49" t="n">
+      <c r="E9" s="50" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
-      <c r="F9" s="47" t="n">
+      <c r="F9" s="48" t="n">
         <f aca="false">(0.1277+0.1276+0.1272)/3</f>
         <v>0.1275</v>
       </c>
-      <c r="G9" s="48" t="n">
+      <c r="G9" s="49" t="n">
         <f aca="false">(0.1109+0.1114+0.1119)/3</f>
         <v>0.1114</v>
       </c>
-      <c r="H9" s="49" t="n">
+      <c r="H9" s="50" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
-      <c r="I9" s="47" t="n">
+      <c r="I9" s="48" t="n">
         <f aca="false">(0.1408)/1</f>
         <v>0.1408</v>
       </c>
-      <c r="J9" s="48"/>
-      <c r="K9" s="49" t="n">
+      <c r="J9" s="49"/>
+      <c r="K9" s="50" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
-      <c r="L9" s="50" t="n">
+      <c r="L9" s="51" t="n">
         <v>0.1255</v>
       </c>
-      <c r="M9" s="48"/>
-      <c r="N9" s="51" t="n">
+      <c r="M9" s="49"/>
+      <c r="N9" s="52" t="n">
         <v>0.0121</v>
       </c>
       <c r="O9" s="0" t="s">
@@ -2063,8 +2064,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="47"/>
+      <c r="B10" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="44" t="n">
@@ -2100,11 +2101,11 @@
         <f aca="false">(0.0925+0.0919)/2</f>
         <v>0.0922</v>
       </c>
-      <c r="L10" s="52" t="n">
+      <c r="L10" s="53" t="n">
         <v>0.1578</v>
       </c>
       <c r="M10" s="45"/>
-      <c r="N10" s="53" t="n">
+      <c r="N10" s="54" t="n">
         <v>0.0837</v>
       </c>
       <c r="O10" s="0" t="s">
@@ -2121,14 +2122,14 @@
       <c r="H11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -2140,53 +2141,53 @@
       <c r="H12" s="0" t="n">
         <v>10.8</v>
       </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="35"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="34"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="38" t="s">
+      <c r="O13" s="37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36"/>
-      <c r="B16" s="35" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="O16" s="38" t="s">
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="O16" s="37" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="O17" s="37" t="s">
         <v>20</v>
       </c>
       <c r="Q17" s="0" t="s">
@@ -2194,11 +2195,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="38" t="s">
+      <c r="O18" s="37" t="s">
         <v>20</v>
       </c>
       <c r="Q18" s="0" t="s">
@@ -2206,21 +2207,21 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="36" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36"/>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="34" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="35" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -2228,7 +2229,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="35" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -2236,27 +2237,27 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36"/>
+      <c r="A24" s="35"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36"/>
-      <c r="B26" s="35" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="34" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="0" t="s">
@@ -2264,10 +2265,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="33" t="s">
         <v>42</v>
       </c>
       <c r="H28" s="0" t="s">
@@ -2275,18 +2276,18 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="33" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="33" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2332,84 +2333,84 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="48" t="n">
+      <c r="B2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.246372705070837</v>
       </c>
-      <c r="H2" s="48" t="n">
+      <c r="H2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.299719963743936</v>
       </c>
-      <c r="N2" s="48" t="n">
+      <c r="N2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.0522741810074534</v>
       </c>
-      <c r="T2" s="48" t="n">
+      <c r="T2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0539992181013351</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8646,7 +8647,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>0.23</v>
@@ -8670,7 +8671,7 @@
         <v>64</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -8690,7 +8691,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>0.26</v>
@@ -8720,7 +8721,7 @@
         <v>73</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -8740,7 +8741,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>0.2</v>
@@ -8770,7 +8771,7 @@
         <v>85</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -15062,17 +15063,17 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S305" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S306" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S307" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -15101,85 +15102,85 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="48" t="n">
+      <c r="B2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.327147963466075</v>
       </c>
-      <c r="H2" s="48" t="n">
+      <c r="H2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.319366602303163</v>
       </c>
-      <c r="N2" s="48" t="n">
+      <c r="N2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.104029611169128</v>
       </c>
-      <c r="T2" s="48" t="n">
+      <c r="T2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0365467584821904</v>
       </c>
-      <c r="U2" s="48"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21416,7 +21417,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -21434,7 +21435,7 @@
         <v>570</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -21454,7 +21455,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -21472,7 +21473,7 @@
         <v>546</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -21492,7 +21493,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -21510,7 +21511,7 @@
         <v>553</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -27802,26 +27803,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -27850,85 +27851,85 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="48" t="n">
+      <c r="B2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.353749402826351</v>
       </c>
-      <c r="H2" s="48" t="n">
+      <c r="H2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.279436534237502</v>
       </c>
-      <c r="N2" s="48" t="n">
+      <c r="N2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.100521589720816</v>
       </c>
-      <c r="T2" s="48" t="n">
+      <c r="T2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0494590627578899</v>
       </c>
-      <c r="U2" s="48"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34165,7 +34166,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -34183,7 +34184,7 @@
         <v>3360</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -34203,7 +34204,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -34221,7 +34222,7 @@
         <v>3172</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -34241,7 +34242,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -34259,7 +34260,7 @@
         <v>3227</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -40551,26 +40552,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -40599,24 +40600,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="0" t="n">
         <f aca="false">COUNTIF(H4:H103,"=1")</f>
         <v>72</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="48" t="n">
+      <c r="B2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.351121061743667</v>
       </c>
@@ -40624,7 +40625,7 @@
         <f aca="false">COUNTIF(B4:B103,"=0")</f>
         <v>23</v>
       </c>
-      <c r="H2" s="48" t="n">
+      <c r="H2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.278690339903548</v>
       </c>
@@ -40632,64 +40633,64 @@
         <f aca="false">COUNTIF(H4:H103,"=0")</f>
         <v>10</v>
       </c>
-      <c r="N2" s="48" t="n">
+      <c r="N2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.0802869852466762</v>
       </c>
-      <c r="T2" s="48" t="n">
+      <c r="T2" s="49" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0566054178796812</v>
       </c>
-      <c r="U2" s="48"/>
+      <c r="U2" s="49"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46926,7 +46927,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -46944,7 +46945,7 @@
         <v>3281</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -46964,7 +46965,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -46982,7 +46983,7 @@
         <v>3285</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -47002,7 +47003,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -47020,7 +47021,7 @@
         <v>3161</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -53312,26 +53313,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update produced graphs and result files
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -585,7 +585,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -670,7 +670,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -691,10 +691,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -886,7 +882,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M7:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1200,53 +1196,53 @@
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11" t="n">
-        <f aca="false">(0.4325+0.4169+0.4658)/3</f>
-        <v>0.4384</v>
+      <c r="C7" s="22" t="n">
+        <f aca="false">(0.6112+0.6304+0.6373)/3</f>
+        <v>0.6263</v>
       </c>
       <c r="D7" s="12" t="n">
-        <f aca="false">(0.4404+0.448+0.4405)/3</f>
-        <v>0.442966666666667</v>
+        <f aca="false">(0.6441+0.6473+0.653)/3</f>
+        <v>0.648133333333333</v>
       </c>
       <c r="E7" s="13" t="n">
-        <f aca="false">(0.0195+0.0203+0.02)/3</f>
-        <v>0.0199333333333333</v>
-      </c>
-      <c r="F7" s="27" t="n">
-        <f aca="false">(0.4323+0.3849+0.3826)/3</f>
-        <v>0.399933333333333</v>
+        <f aca="false">(0.0218+0.0203+0.0221)/3</f>
+        <v>0.0214</v>
+      </c>
+      <c r="F7" s="21" t="n">
+        <f aca="false">(0.6396+0.6221+0.6312)/3</f>
+        <v>0.630966666666667</v>
       </c>
       <c r="G7" s="23" t="n">
-        <f aca="false">(0.4254+0.4457+0.4062)/3</f>
-        <v>0.425766666666667</v>
-      </c>
-      <c r="H7" s="28" t="n">
-        <f aca="false">(0.0209+0.0207+0.0214)/3</f>
-        <v>0.021</v>
-      </c>
-      <c r="I7" s="27" t="n">
-        <f aca="false">(0.3599+0.3714)/2</f>
-        <v>0.36565</v>
+        <f aca="false">(0.6344+0.6545+0.6652)/3</f>
+        <v>0.651366666666667</v>
+      </c>
+      <c r="H7" s="27" t="n">
+        <f aca="false">(0.0264+0.0266+0.0259)/3</f>
+        <v>0.0263</v>
+      </c>
+      <c r="I7" s="21" t="n">
+        <f aca="false">(0.5581+0.5766)/2</f>
+        <v>0.56735</v>
       </c>
       <c r="J7" s="23" t="n">
-        <f aca="false">(0.3698+0.3561)/2</f>
-        <v>0.36295</v>
-      </c>
-      <c r="K7" s="28" t="n">
-        <f aca="false">(0.0259+0.025)/2</f>
+        <f aca="false">(0.5855+0.5623)/2</f>
+        <v>0.5739</v>
+      </c>
+      <c r="K7" s="27" t="n">
+        <f aca="false">(0.0254+0.0255)/2</f>
         <v>0.02545</v>
       </c>
-      <c r="L7" s="27" t="n">
-        <f aca="false">(0.3481+0.3196)/2</f>
-        <v>0.33385</v>
+      <c r="L7" s="21" t="n">
+        <f aca="false">(0.5497+0.5899)/2</f>
+        <v>0.5698</v>
       </c>
       <c r="M7" s="23" t="n">
-        <f aca="false">(0.3444+0.3257)/2</f>
-        <v>0.33505</v>
-      </c>
-      <c r="N7" s="28" t="n">
-        <f aca="false">(0.0209+0.0214)/2</f>
-        <v>0.02115</v>
+        <f aca="false">(0.5392+0.5216)/2</f>
+        <v>0.5304</v>
+      </c>
+      <c r="N7" s="27" t="n">
+        <f aca="false">(0.0269+0.0266)/2</f>
+        <v>0.02675</v>
       </c>
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
@@ -1254,56 +1250,56 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="15" t="n">
-        <f aca="false">(0.2376+0.2338+0.235)/3</f>
-        <v>0.235466666666667</v>
+        <f aca="false">(0.3817+0.3833+0.3718)/3</f>
+        <v>0.378933333333333</v>
       </c>
       <c r="D8" s="16" t="n">
-        <f aca="false">(0.2633+0.2577+0.2631)/3</f>
-        <v>0.261366666666667</v>
+        <f aca="false">(0.407+0.4018+0.412)/3</f>
+        <v>0.406933333333333</v>
       </c>
       <c r="E8" s="17" t="n">
-        <f aca="false">(0.1143+0.1132+0.1152)/3</f>
-        <v>0.114233333333333</v>
+        <f aca="false">(0.1191+0.1188+0.1179)/3</f>
+        <v>0.1186</v>
       </c>
       <c r="F8" s="15" t="n">
-        <f aca="false">(0.265+0.2708+0.2727)/3</f>
-        <v>0.2695</v>
+        <f aca="false">(0.3664+0.3685+0.3734)/3</f>
+        <v>0.369433333333333</v>
       </c>
       <c r="G8" s="16" t="n">
-        <f aca="false">(0.2735+0.2845+0.2889)/3</f>
-        <v>0.2823</v>
+        <f aca="false">(0.3681+0.3662+0.3614)/3</f>
+        <v>0.365233333333333</v>
       </c>
       <c r="H8" s="17" t="n">
-        <f aca="false">(0.1134+0.1143+0.1151)/3</f>
-        <v>0.114266666666667</v>
+        <f aca="false">(0.1166+0.1165+0.117)/3</f>
+        <v>0.1167</v>
       </c>
       <c r="I8" s="15" t="n">
-        <f aca="false">(0.232+0.2333)/2</f>
-        <v>0.23265</v>
+        <f aca="false">(0.3306+0.3313)/2</f>
+        <v>0.33095</v>
       </c>
       <c r="J8" s="16" t="n">
-        <f aca="false">(0.2377+0.2336)/2</f>
-        <v>0.23565</v>
+        <f aca="false">(0.3347+0.3299)/2</f>
+        <v>0.3323</v>
       </c>
       <c r="K8" s="17" t="n">
-        <f aca="false">(0.1066+0.1064)/2</f>
-        <v>0.1065</v>
+        <f aca="false">(0.104+0.1046)/2</f>
+        <v>0.1043</v>
       </c>
       <c r="L8" s="15" t="n">
-        <f aca="false">(0.2254+0.2285)/2</f>
-        <v>0.22695</v>
+        <f aca="false">(0.338+0.34)/2</f>
+        <v>0.339</v>
       </c>
       <c r="M8" s="16" t="n">
-        <f aca="false">(0.2164+0.292)/2</f>
-        <v>0.2542</v>
+        <f aca="false">(0.3302+0.3276)/2</f>
+        <v>0.3289</v>
       </c>
       <c r="N8" s="17" t="n">
-        <f aca="false">(0.099+0.0987)/2</f>
-        <v>0.09885</v>
+        <f aca="false">(0.103+0.103)/2</f>
+        <v>0.103</v>
       </c>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
@@ -1316,7 +1312,7 @@
       <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="27" t="n">
+      <c r="C9" s="21" t="n">
         <f aca="false">(0.3587+0.3632+0.3573)/3</f>
         <v>0.359733333333333</v>
       </c>
@@ -1324,11 +1320,11 @@
         <f aca="false">(0.3498+0.3479+0.3496)/3</f>
         <v>0.3491</v>
       </c>
-      <c r="E9" s="28" t="n">
+      <c r="E9" s="27" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
-      <c r="F9" s="27" t="n">
+      <c r="F9" s="21" t="n">
         <f aca="false">(0.4789+0.4773+0.4784)/3</f>
         <v>0.4782</v>
       </c>
@@ -1336,11 +1332,11 @@
         <f aca="false">(0.4779+0.4776+0.4793)/3</f>
         <v>0.478266666666667</v>
       </c>
-      <c r="H9" s="28" t="n">
+      <c r="H9" s="27" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
-      <c r="I9" s="27" t="n">
+      <c r="I9" s="21" t="n">
         <f aca="false">(0.5451+0.5452)/2</f>
         <v>0.54515</v>
       </c>
@@ -1348,11 +1344,11 @@
         <f aca="false">(0.5451+0.5456)/2</f>
         <v>0.54535</v>
       </c>
-      <c r="K9" s="28" t="n">
+      <c r="K9" s="27" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
-      <c r="L9" s="27" t="n">
+      <c r="L9" s="21" t="n">
         <f aca="false">(0.5042+0.508)/2</f>
         <v>0.5061</v>
       </c>
@@ -1360,7 +1356,7 @@
         <f aca="false">(0.5145+0.5146)/2</f>
         <v>0.51455</v>
       </c>
-      <c r="N9" s="28" t="n">
+      <c r="N9" s="27" t="n">
         <f aca="false">(0.0239+0.0239)/2</f>
         <v>0.0239</v>
       </c>
@@ -1426,63 +1422,63 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="34"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="37" t="s">
+      <c r="O13" s="36" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35"/>
-      <c r="B16" s="34" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="O16" s="37" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="O16" s="36" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="37" t="s">
+      <c r="O17" s="36" t="s">
         <v>20</v>
       </c>
       <c r="Q17" s="0" t="s">
@@ -1490,11 +1486,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="37" t="s">
+      <c r="O18" s="36" t="s">
         <v>20</v>
       </c>
       <c r="Q18" s="0" t="s">
@@ -1502,21 +1498,21 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="35"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -1524,7 +1520,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -1532,27 +1528,27 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35"/>
+      <c r="A24" s="34"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35"/>
-      <c r="B26" s="34" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="33" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="32" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="0" t="s">
@@ -1560,10 +1556,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>42</v>
       </c>
       <c r="H28" s="0" t="s">
@@ -1571,18 +1567,18 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="32" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1616,7 +1612,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="M7:M8 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1706,254 +1702,254 @@
       <c r="Q2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="39" t="n">
+      <c r="C3" s="38" t="n">
         <f aca="false">(0.3606+0.3668+0.3843)/3</f>
         <v>0.370566666666667</v>
       </c>
-      <c r="D3" s="40" t="n">
+      <c r="D3" s="39" t="n">
         <f aca="false">(0.3432+0.331+0.3215)/3</f>
         <v>0.3319</v>
       </c>
-      <c r="E3" s="40" t="n">
+      <c r="E3" s="39" t="n">
         <f aca="false">(0.0224+0.0224+0.0237)/3</f>
         <v>0.0228333333333333</v>
       </c>
-      <c r="F3" s="39" t="n">
+      <c r="F3" s="38" t="n">
         <f aca="false">(0.5904+0.6326+0.6324)/3</f>
         <v>0.618466666666667</v>
       </c>
-      <c r="G3" s="40" t="n">
+      <c r="G3" s="39" t="n">
         <f aca="false">(0.3918+0.4014+0.3884)/3</f>
         <v>0.393866666666667</v>
       </c>
-      <c r="H3" s="41" t="n">
+      <c r="H3" s="40" t="n">
         <f aca="false">(0.0194+0.0194+0.0191)/3</f>
         <v>0.0193</v>
       </c>
-      <c r="I3" s="39" t="n">
+      <c r="I3" s="38" t="n">
         <f aca="false">(0.7877+0.7969)/2</f>
         <v>0.7923</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="41" t="n">
+      <c r="J3" s="39"/>
+      <c r="K3" s="40" t="n">
         <f aca="false">(0.0181+0.0175)/2</f>
         <v>0.0178</v>
       </c>
-      <c r="L3" s="42" t="n">
+      <c r="L3" s="41" t="n">
         <v>0.7585</v>
       </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41" t="n">
+      <c r="M3" s="39"/>
+      <c r="N3" s="40" t="n">
         <f aca="false">(0.0195+0.0186)/2</f>
         <v>0.01905</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="38"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="44" t="n">
+      <c r="C4" s="43" t="n">
         <f aca="false">(0.2272+0.2116+0.22)/3</f>
         <v>0.2196</v>
       </c>
-      <c r="D4" s="45" t="n">
+      <c r="D4" s="44" t="n">
         <f aca="false">(0.8626+0.8314+0.8503)/3</f>
         <v>0.8481</v>
       </c>
-      <c r="E4" s="45" t="n">
+      <c r="E4" s="44" t="n">
         <f aca="false">(0.1181+0.1143+0.1121)/3</f>
         <v>0.114833333333333</v>
       </c>
-      <c r="F4" s="44" t="n">
+      <c r="F4" s="43" t="n">
         <f aca="false">(0.3011+0.3014+0.3215)/3</f>
         <v>0.308</v>
       </c>
-      <c r="G4" s="45" t="n">
+      <c r="G4" s="44" t="n">
         <f aca="false">(0.9691+0.9503+0.9682)/3</f>
         <v>0.962533333333333</v>
       </c>
-      <c r="H4" s="46" t="n">
+      <c r="H4" s="45" t="n">
         <f aca="false">(0.1134+0.1125+0.1133)/3</f>
         <v>0.113066666666667</v>
       </c>
-      <c r="I4" s="44" t="n">
+      <c r="I4" s="43" t="n">
         <f aca="false">(0.3189+0.3365)/2</f>
         <v>0.3277</v>
       </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="46" t="n">
+      <c r="J4" s="44"/>
+      <c r="K4" s="45" t="n">
         <f aca="false">(0.1034+0.1005)/2</f>
         <v>0.10195</v>
       </c>
-      <c r="L4" s="45" t="n">
+      <c r="L4" s="44" t="n">
         <f aca="false">(0.3255+0.3285)/2</f>
         <v>0.327</v>
       </c>
-      <c r="M4" s="45"/>
-      <c r="N4" s="46" t="n">
+      <c r="M4" s="44"/>
+      <c r="N4" s="45" t="n">
         <f aca="false">(0.0985+0.0986)/2</f>
         <v>0.09855</v>
       </c>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="46" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="40" t="n">
+      <c r="C5" s="39" t="n">
         <f aca="false">(0.5514+0.5606+0.5368)/3</f>
         <v>0.5496</v>
       </c>
-      <c r="D5" s="40" t="n">
+      <c r="D5" s="39" t="n">
         <f aca="false">(0.4411+0.4414+0.4382)/3</f>
         <v>0.440233333333333</v>
       </c>
-      <c r="E5" s="40" t="n">
+      <c r="E5" s="39" t="n">
         <f aca="false">(0.026+0.0242+0.0238)/3</f>
         <v>0.0246666666666667</v>
       </c>
-      <c r="F5" s="39" t="n">
+      <c r="F5" s="38" t="n">
         <f aca="false">(0.6699+0.6706+0.6927)/3</f>
         <v>0.677733333333333</v>
       </c>
-      <c r="G5" s="40" t="n">
+      <c r="G5" s="39" t="n">
         <f aca="false">(0.4393+0.4335+0.4325)/3</f>
         <v>0.4351</v>
       </c>
-      <c r="H5" s="41" t="n">
+      <c r="H5" s="40" t="n">
         <f aca="false">(0.0238+0.0237+0.0242)/3</f>
         <v>0.0239</v>
       </c>
-      <c r="I5" s="39" t="n">
+      <c r="I5" s="38" t="n">
         <f aca="false">(0.8098+0.8098)/2</f>
         <v>0.8098</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="41" t="n">
+      <c r="J5" s="39"/>
+      <c r="K5" s="40" t="n">
         <f aca="false">(0.0234+0.0232)/2</f>
         <v>0.0233</v>
       </c>
-      <c r="L5" s="39" t="n">
+      <c r="L5" s="38" t="n">
         <f aca="false">(0.7684+0.755)/2</f>
         <v>0.7617</v>
       </c>
-      <c r="M5" s="40"/>
-      <c r="N5" s="41" t="n">
+      <c r="M5" s="39"/>
+      <c r="N5" s="40" t="n">
         <f aca="false">(0.0252+0.0244)/2</f>
         <v>0.0248</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="45" t="n">
+      <c r="C6" s="44" t="n">
         <f aca="false">(0.4186+0.4008+0.4108)/3</f>
         <v>0.410066666666667</v>
       </c>
-      <c r="D6" s="45" t="n">
+      <c r="D6" s="44" t="n">
         <f aca="false">(0.8625+0.8393+0.8551)/3</f>
         <v>0.8523</v>
       </c>
-      <c r="E6" s="45" t="n">
+      <c r="E6" s="44" t="n">
         <f aca="false">(0.1169+0.1121+0.1149)/3</f>
         <v>0.114633333333333</v>
       </c>
-      <c r="F6" s="44" t="n">
+      <c r="F6" s="43" t="n">
         <f aca="false">(0.5177+0.5266+0.5236)/3</f>
         <v>0.522633333333333</v>
       </c>
-      <c r="G6" s="45" t="n">
+      <c r="G6" s="44" t="n">
         <f aca="false">(0.9399+0.9168+0.9156)/3</f>
         <v>0.9241</v>
       </c>
-      <c r="H6" s="46" t="n">
+      <c r="H6" s="45" t="n">
         <f aca="false">(0.1146+0.1146+0.115)/3</f>
         <v>0.114733333333333</v>
       </c>
-      <c r="I6" s="44" t="n">
+      <c r="I6" s="43" t="n">
         <f aca="false">(0.5984+0.5822)/2</f>
         <v>0.5903</v>
       </c>
-      <c r="J6" s="45"/>
-      <c r="K6" s="46" t="n">
+      <c r="J6" s="44"/>
+      <c r="K6" s="45" t="n">
         <f aca="false">(0.1011+0.1012)/2</f>
         <v>0.10115</v>
       </c>
-      <c r="L6" s="44" t="n">
+      <c r="L6" s="43" t="n">
         <f aca="false">(0.6002+0.6068)/2</f>
         <v>0.6035</v>
       </c>
-      <c r="M6" s="45"/>
-      <c r="N6" s="46" t="n">
+      <c r="M6" s="44"/>
+      <c r="N6" s="45" t="n">
         <f aca="false">(0.0999+0.1007)/2</f>
         <v>0.1003</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="46" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="39" t="n">
+      <c r="C7" s="38" t="n">
         <f aca="false">(0.3225+0.3037)/2</f>
         <v>0.3131</v>
       </c>
-      <c r="D7" s="40" t="n">
+      <c r="D7" s="39" t="n">
         <f aca="false">(0.2421+0.2415+0.2214)/3</f>
         <v>0.235</v>
       </c>
-      <c r="E7" s="41" t="n">
+      <c r="E7" s="40" t="n">
         <f aca="false">(0.0195+0.0203+0.02)/3</f>
         <v>0.0199333333333333</v>
       </c>
-      <c r="F7" s="48" t="n">
+      <c r="F7" s="47" t="n">
         <f aca="false">(0.3343+0.3376+0.3375)/3</f>
         <v>0.336466666666667</v>
       </c>
-      <c r="G7" s="49" t="n">
+      <c r="G7" s="48" t="n">
         <f aca="false">(0.2274+0.2273+0.2291)/3</f>
         <v>0.227933333333333</v>
       </c>
-      <c r="H7" s="50" t="n">
+      <c r="H7" s="49" t="n">
         <f aca="false">(0.0209+0.0207+0.0214)/3</f>
         <v>0.021</v>
       </c>
-      <c r="I7" s="48" t="n">
+      <c r="I7" s="47" t="n">
         <f aca="false">(0.3418+0.3334+0.3179)/3</f>
         <v>0.331033333333333</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="50" t="n">
+      <c r="J7" s="48"/>
+      <c r="K7" s="49" t="n">
         <f aca="false">(0.0319+0.0309+0.031)/3</f>
         <v>0.0312666666666667</v>
       </c>
-      <c r="L7" s="48" t="n">
+      <c r="L7" s="47" t="n">
         <f aca="false">(0.2997+0.3176+0.3301)/3</f>
         <v>0.3158</v>
       </c>
-      <c r="M7" s="49"/>
-      <c r="N7" s="50" t="n">
+      <c r="M7" s="48"/>
+      <c r="N7" s="49" t="n">
         <f aca="false">(0.0209+0.0214)/2</f>
         <v>0.02115</v>
       </c>
@@ -1962,49 +1958,49 @@
       <c r="Q7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47"/>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="46"/>
+      <c r="B8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="44" t="n">
+      <c r="C8" s="43" t="n">
         <f aca="false">(0.1988+0.1939+0.2009)/3</f>
         <v>0.197866666666667</v>
       </c>
-      <c r="D8" s="45" t="n">
+      <c r="D8" s="44" t="n">
         <f aca="false">(0.4076+0.4322+0.4131)/3</f>
         <v>0.417633333333333</v>
       </c>
-      <c r="E8" s="46" t="n">
+      <c r="E8" s="45" t="n">
         <f aca="false">(0.1143+0.1132+0.1152)/3</f>
         <v>0.114233333333333</v>
       </c>
-      <c r="F8" s="44" t="n">
+      <c r="F8" s="43" t="n">
         <f aca="false">(0.1904+0.192+0.1935)/3</f>
         <v>0.191966666666667</v>
       </c>
-      <c r="G8" s="45" t="n">
+      <c r="G8" s="44" t="n">
         <f aca="false">(0.3899+0.4101+0.4039)/3</f>
         <v>0.4013</v>
       </c>
-      <c r="H8" s="46" t="n">
+      <c r="H8" s="45" t="n">
         <f aca="false">(0.1134+0.1143+0.1151)/3</f>
         <v>0.114266666666667</v>
       </c>
-      <c r="I8" s="44" t="n">
+      <c r="I8" s="43" t="n">
         <f aca="false">(0.1659+0.1608+0.1658)/3</f>
         <v>0.164166666666667</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="46" t="n">
+      <c r="J8" s="44"/>
+      <c r="K8" s="45" t="n">
         <f aca="false">(0.1062+0.1066+0.1064)/3</f>
         <v>0.1064</v>
       </c>
-      <c r="L8" s="44" t="n">
+      <c r="L8" s="43" t="n">
         <f aca="false">(0.1647+0.164)/2</f>
         <v>0.16435</v>
       </c>
-      <c r="M8" s="45"/>
-      <c r="N8" s="46" t="n">
+      <c r="M8" s="44"/>
+      <c r="N8" s="45" t="n">
         <f aca="false">(0.099+0.0987)/2</f>
         <v>0.09885</v>
       </c>
@@ -2013,50 +2009,50 @@
       <c r="Q8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="46" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="48" t="n">
+      <c r="C9" s="47" t="n">
         <f aca="false">(0.1062+0.1091+0.1051)/3</f>
         <v>0.1068</v>
       </c>
-      <c r="D9" s="49" t="n">
+      <c r="D9" s="48" t="n">
         <f aca="false">(0.085+0.0874+0.0856)/3</f>
         <v>0.086</v>
       </c>
-      <c r="E9" s="50" t="n">
+      <c r="E9" s="49" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
-      <c r="F9" s="48" t="n">
+      <c r="F9" s="47" t="n">
         <f aca="false">(0.1277+0.1276+0.1272)/3</f>
         <v>0.1275</v>
       </c>
-      <c r="G9" s="49" t="n">
+      <c r="G9" s="48" t="n">
         <f aca="false">(0.1109+0.1114+0.1119)/3</f>
         <v>0.1114</v>
       </c>
-      <c r="H9" s="50" t="n">
+      <c r="H9" s="49" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
-      <c r="I9" s="48" t="n">
+      <c r="I9" s="47" t="n">
         <f aca="false">(0.1408)/1</f>
         <v>0.1408</v>
       </c>
-      <c r="J9" s="49"/>
-      <c r="K9" s="50" t="n">
+      <c r="J9" s="48"/>
+      <c r="K9" s="49" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
-      <c r="L9" s="51" t="n">
+      <c r="L9" s="50" t="n">
         <v>0.1255</v>
       </c>
-      <c r="M9" s="49"/>
-      <c r="N9" s="52" t="n">
+      <c r="M9" s="48"/>
+      <c r="N9" s="51" t="n">
         <v>0.0121</v>
       </c>
       <c r="O9" s="0" t="s">
@@ -2064,48 +2060,48 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="47"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="44" t="n">
+      <c r="C10" s="43" t="n">
         <f aca="false">(0.1401+0.1378+0.1374)/3</f>
         <v>0.138433333333333</v>
       </c>
-      <c r="D10" s="45" t="n">
+      <c r="D10" s="44" t="n">
         <f aca="false">(0.2803+0.2808+0.2771)/3</f>
         <v>0.2794</v>
       </c>
-      <c r="E10" s="46" t="n">
+      <c r="E10" s="45" t="n">
         <f aca="false">(0.1026+0.1017+0.1048)/3</f>
         <v>0.103033333333333</v>
       </c>
-      <c r="F10" s="44" t="n">
+      <c r="F10" s="43" t="n">
         <f aca="false">(0.1577+0.1582+0.1566)/3</f>
         <v>0.1575</v>
       </c>
-      <c r="G10" s="45" t="n">
+      <c r="G10" s="44" t="n">
         <f aca="false">(0.3699+0.3739+0.3682)/3</f>
         <v>0.370666666666667</v>
       </c>
-      <c r="H10" s="46" t="n">
+      <c r="H10" s="45" t="n">
         <f aca="false">(0.1071+0.1084+0.1071)/3</f>
         <v>0.107533333333333</v>
       </c>
-      <c r="I10" s="44" t="n">
+      <c r="I10" s="43" t="n">
         <f aca="false">(0.1756)/1</f>
         <v>0.1756</v>
       </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="46" t="n">
+      <c r="J10" s="44"/>
+      <c r="K10" s="45" t="n">
         <f aca="false">(0.0925+0.0919)/2</f>
         <v>0.0922</v>
       </c>
-      <c r="L10" s="53" t="n">
+      <c r="L10" s="52" t="n">
         <v>0.1578</v>
       </c>
-      <c r="M10" s="45"/>
-      <c r="N10" s="54" t="n">
+      <c r="M10" s="44"/>
+      <c r="N10" s="53" t="n">
         <v>0.0837</v>
       </c>
       <c r="O10" s="0" t="s">
@@ -2122,14 +2118,14 @@
       <c r="H11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -2141,53 +2137,53 @@
       <c r="H12" s="0" t="n">
         <v>10.8</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="34"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="37" t="s">
+      <c r="O13" s="36" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35"/>
-      <c r="B16" s="34" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="O16" s="37" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="O16" s="36" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="O17" s="37" t="s">
+      <c r="O17" s="36" t="s">
         <v>20</v>
       </c>
       <c r="Q17" s="0" t="s">
@@ -2195,11 +2191,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="37" t="s">
+      <c r="O18" s="36" t="s">
         <v>20</v>
       </c>
       <c r="Q18" s="0" t="s">
@@ -2207,21 +2203,21 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="35"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="33" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -2229,7 +2225,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -2237,27 +2233,27 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35"/>
+      <c r="A24" s="34"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35"/>
-      <c r="B26" s="34" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="33" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="32" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="0" t="s">
@@ -2265,10 +2261,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="32" t="s">
         <v>42</v>
       </c>
       <c r="H28" s="0" t="s">
@@ -2276,18 +2272,18 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="33" t="s">
+      <c r="B30" s="32" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2323,7 +2319,7 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="M7:M8 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2346,19 +2342,19 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="49" t="n">
+      <c r="B2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.246372705070837</v>
       </c>
-      <c r="H2" s="49" t="n">
+      <c r="H2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.299719963743936</v>
       </c>
-      <c r="N2" s="49" t="n">
+      <c r="N2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.0522741810074534</v>
       </c>
-      <c r="T2" s="49" t="n">
+      <c r="T2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0539992181013351</v>
       </c>
@@ -15095,7 +15091,7 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="M7:M8 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15115,23 +15111,23 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="49" t="n">
+      <c r="B2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.327147963466075</v>
       </c>
-      <c r="H2" s="49" t="n">
+      <c r="H2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.319366602303163</v>
       </c>
-      <c r="N2" s="49" t="n">
+      <c r="N2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.104029611169128</v>
       </c>
-      <c r="T2" s="49" t="n">
+      <c r="T2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0365467584821904</v>
       </c>
-      <c r="U2" s="49"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
@@ -27844,7 +27840,7 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+      <selection pane="topLeft" activeCell="T2" activeCellId="1" sqref="M7:M8 T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27864,23 +27860,23 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="49" t="n">
+      <c r="B2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.353749402826351</v>
       </c>
-      <c r="H2" s="49" t="n">
+      <c r="H2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.279436534237502</v>
       </c>
-      <c r="N2" s="49" t="n">
+      <c r="N2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.100521589720816</v>
       </c>
-      <c r="T2" s="49" t="n">
+      <c r="T2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0494590627578899</v>
       </c>
-      <c r="U2" s="49"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
@@ -40593,7 +40589,7 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H303" activeCellId="0" sqref="H303"/>
+      <selection pane="topLeft" activeCell="H303" activeCellId="1" sqref="M7:M8 H303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40617,7 +40613,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="49" t="n">
+      <c r="B2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(B4:B303)</f>
         <v>0.351121061743667</v>
       </c>
@@ -40625,7 +40621,7 @@
         <f aca="false">COUNTIF(B4:B103,"=0")</f>
         <v>23</v>
       </c>
-      <c r="H2" s="49" t="n">
+      <c r="H2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(H4:H303)</f>
         <v>0.278690339903548</v>
       </c>
@@ -40633,15 +40629,15 @@
         <f aca="false">COUNTIF(H4:H103,"=0")</f>
         <v>10</v>
       </c>
-      <c r="N2" s="49" t="n">
+      <c r="N2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(N4:N303)</f>
         <v>0.0802869852466762</v>
       </c>
-      <c r="T2" s="49" t="n">
+      <c r="T2" s="48" t="n">
         <f aca="false">_xlfn.STDEV.P(T4:T303)</f>
         <v>0.0566054178796812</v>
       </c>
-      <c r="U2" s="49"/>
+      <c r="U2" s="48"/>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">

</xml_diff>

<commit_message>
Weekly+Daily initial with solar results
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="128">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -48,13 +48,13 @@
     <t xml:space="preserve">Case</t>
   </si>
   <si>
-    <t xml:space="preserve">1 L / C</t>
+    <t xml:space="preserve">LPC</t>
   </si>
   <si>
-    <t xml:space="preserve">1 L / P</t>
+    <t xml:space="preserve">LPP</t>
   </si>
   <si>
-    <t xml:space="preserve">1 L</t>
+    <t xml:space="preserve">AOL</t>
   </si>
   <si>
     <t xml:space="preserve">MLP</t>
@@ -96,10 +96,10 @@
     <t xml:space="preserve">Blockchain data analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">Stage 1 establishes the likelihood to extract a user's dataset of transactions for stage 2</t>
+    <t xml:space="preserve">Stage 1 establishes the likelihood to extract a user's dataset of transactions for stage 2.</t>
   </si>
   <si>
-    <t xml:space="preserve">Investigate classification methods: MLP, CNN, RFC, KNN</t>
+    <t xml:space="preserve">Investigate classification methods: MLP, CNN, RFC, KNN.</t>
   </si>
   <si>
     <t xml:space="preserve">What's the likelihood one can see a transaction and pick the customer or postcode?</t>
@@ -117,19 +117,19 @@
     <t xml:space="preserve">Include off-chain weather data</t>
   </si>
   <si>
-    <t xml:space="preserve">Stage 2 measures the chance an attacker can find the customer's location from their dataset and solar data</t>
+    <t xml:space="preserve">Stage 2 measures the chance an attacker can find the customer's location from their dataset and solar data.</t>
   </si>
   <si>
     <t xml:space="preserve">2a</t>
   </si>
   <si>
-    <t xml:space="preserve">Investigate approaches to combine a user data set with solar data to reveal postcode.</t>
+    <t xml:space="preserve">Investigate classification methods with additional solar data added: CNN, RFC.</t>
   </si>
   <si>
     <t xml:space="preserve">2b</t>
   </si>
   <si>
-    <t xml:space="preserve">Explore whether solar data has an impact on stage 1 analysis.</t>
+    <t xml:space="preserve">Investigate whether separate cointegration and correlation analysis can link.</t>
   </si>
   <si>
     <t xml:space="preserve">Stage 3</t>
@@ -138,13 +138,13 @@
     <t xml:space="preserve">Obfuscation methods</t>
   </si>
   <si>
-    <t xml:space="preserve">Stage 3 investigates methods to increase privacy and reduce the effectiveness of stage 1 and 2</t>
+    <t xml:space="preserve">Stage 3 investigates methods to increase privacy and reduce the effectiveness of stage 1 and 2.</t>
   </si>
   <si>
     <t xml:space="preserve">3a</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiple PKs efficiency</t>
+    <t xml:space="preserve">Multiple PKs and ledgers efficiency.</t>
   </si>
   <si>
     <t xml:space="preserve">1 to n at reasonable intervals</t>
@@ -153,10 +153,58 @@
     <t xml:space="preserve">3b</t>
   </si>
   <si>
-    <t xml:space="preserve">Multiple customers per ledger efficiency</t>
+    <t xml:space="preserve">Transaction obfuscation: random delays and combinations.</t>
   </si>
   <si>
     <t xml:space="preserve">3c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combine best of a and b for a final test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage 1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best case is each customer on an individual ledger with one PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 L / C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 L / P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worst case is all customers on one ledger with new PK per transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage 1 establishes the likelihood to extract a user's dataset of transactions for stage 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigate classification methods: MLP, RF, KNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage 2 measures the chance an attacker can find the customer's location from their dataset and solar data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigate approaches to combine a user data set with solar data to reveal postcode.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explore whether solar data has an impact on stage 1 analysis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage 3 investigates methods to increase privacy and reduce the effectiveness of stage 1 and 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple PKs efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple customers per ledger efficiency</t>
   </si>
   <si>
     <t xml:space="preserve">Timestamp obfuscation: random transaction delays and combinations</t>
@@ -166,21 +214,6 @@
   </si>
   <si>
     <t xml:space="preserve">Combinations of a-c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage 1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best case is each customer on an individual ledger with one PK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Worst case is all customers on one ledger with new PK per transaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigate classification methods: MLP, RF, KNN</t>
   </si>
   <si>
     <t xml:space="preserve">MLP postcode weekly best</t>
@@ -444,7 +477,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +488,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F9D4"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -576,7 +615,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -689,6 +728,30 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="9" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -709,11 +772,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -721,19 +784,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -766,7 +829,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFF6F9D4"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -814,10 +877,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1048576"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="F12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1363,165 +1426,287 @@
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
     </row>
-    <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="28" t="n">
+        <f aca="false">(0.6684+0.6912)/2</f>
+        <v>0.6798</v>
+      </c>
+      <c r="D12" s="28" t="n">
+        <f aca="false">(0.6967+0.6607)/2</f>
+        <v>0.6787</v>
+      </c>
+      <c r="E12" s="28" t="n">
+        <f aca="false">(0.0302+0.0307)/2</f>
+        <v>0.03045</v>
+      </c>
+      <c r="F12" s="29" t="n">
+        <f aca="false">(0.7336)/1</f>
+        <v>0.7336</v>
+      </c>
+      <c r="G12" s="28" t="n">
+        <f aca="false">(0.7158)/1</f>
+        <v>0.7158</v>
+      </c>
+      <c r="H12" s="30" t="n">
+        <f aca="false">(0.0282+0.0286)/2</f>
+        <v>0.0284</v>
+      </c>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="19"/>
+      <c r="B13" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="31" t="n">
+        <f aca="false">(0.5605+0.5406)/2</f>
+        <v>0.55055</v>
+      </c>
+      <c r="D13" s="31" t="n">
+        <f aca="false">(0.5246+0.5207)/2</f>
+        <v>0.52265</v>
+      </c>
+      <c r="E13" s="31" t="n">
+        <f aca="false">(0.1216+0.1192)/2</f>
+        <v>0.1204</v>
+      </c>
+      <c r="F13" s="32" t="n">
+        <f aca="false">(0.6049)/1</f>
+        <v>0.6049</v>
+      </c>
+      <c r="G13" s="31" t="n">
+        <f aca="false">(0.5747)/1</f>
+        <v>0.5747</v>
+      </c>
+      <c r="H13" s="33" t="n">
+        <f aca="false">(0.1194+0.1194)/2</f>
+        <v>0.1194</v>
+      </c>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="29" t="n">
+        <f aca="false">(0.7298+0.7055)/2</f>
+        <v>0.71765</v>
+      </c>
+      <c r="D14" s="28" t="n">
+        <f aca="false">(0.7841+0.8337)/2</f>
+        <v>0.8089</v>
+      </c>
+      <c r="E14" s="30" t="n">
+        <f aca="false">(0.0282+0.0285)/2</f>
+        <v>0.02835</v>
+      </c>
+      <c r="F14" s="29" t="n">
+        <f aca="false">(0.7581+0.7598)/2</f>
+        <v>0.75895</v>
+      </c>
+      <c r="G14" s="28" t="n">
+        <f aca="false">(0.7847+0.7562)/2</f>
+        <v>0.77045</v>
+      </c>
+      <c r="H14" s="30" t="n">
+        <f aca="false">(0.037+0.0369)/2</f>
+        <v>0.03695</v>
+      </c>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="19"/>
+      <c r="B15" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="32" t="n">
+        <f aca="false">(0.5823+0.5715)/2</f>
+        <v>0.5769</v>
+      </c>
+      <c r="D15" s="31" t="n">
+        <f aca="false">(0.5692+0.5583)/2</f>
+        <v>0.56375</v>
+      </c>
+      <c r="E15" s="33" t="n">
+        <f aca="false">(0.1638+0.1647)/2</f>
+        <v>0.16425</v>
+      </c>
+      <c r="F15" s="32" t="n">
+        <f aca="false">(0.5205+0.5217)/2</f>
+        <v>0.5211</v>
+      </c>
+      <c r="G15" s="31" t="n">
+        <f aca="false">(0.5214+0.5275)/2</f>
+        <v>0.52445</v>
+      </c>
+      <c r="H15" s="33" t="n">
+        <f aca="false">(0.1307+0.1299)/2</f>
+        <v>0.1303</v>
+      </c>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
+      <c r="L17" s="35"/>
+      <c r="M17" s="36"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B18" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="O18" s="39" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31" t="s">
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B20" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31"/>
-      <c r="B16" s="30" t="s">
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="37"/>
+      <c r="B21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="O16" s="33" t="s">
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="O21" s="39" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31"/>
-      <c r="B17" s="0" t="s">
+    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="37"/>
+      <c r="B22" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="33" t="s">
+      <c r="O22" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="0" t="s">
+      <c r="Q22" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31"/>
-      <c r="B18" s="0" t="s">
+    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="37"/>
+      <c r="B23" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="33" t="s">
+      <c r="O23" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="Q18" s="0" t="s">
+      <c r="Q23" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="s">
+    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B25" s="38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31"/>
-      <c r="B21" s="30" t="s">
+    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="37"/>
+      <c r="B26" s="36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="s">
+    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B27" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B28" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31" t="s">
+    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="37"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B30" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31"/>
-      <c r="B26" s="30" t="s">
+    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="37"/>
+      <c r="B31" s="36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
+    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B32" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H32" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B33" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B34" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
@@ -1531,6 +1716,8 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1550,7 +1737,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="1" sqref="F12:G13 I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1563,7 +1750,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -1587,7 +1774,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
@@ -1600,40 +1787,40 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
@@ -1679,7 +1866,7 @@
         <f aca="false">(0.0181+0.0175)/2</f>
         <v>0.0178</v>
       </c>
-      <c r="L3" s="34" t="n">
+      <c r="L3" s="40" t="n">
         <v>0.7585</v>
       </c>
       <c r="M3" s="12"/>
@@ -1687,11 +1874,11 @@
         <f aca="false">(0.0195+0.0186)/2</f>
         <v>0.01905</v>
       </c>
-      <c r="O3" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
+      <c r="O3" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
@@ -1740,9 +1927,9 @@
         <f aca="false">(0.0985+0.0986)/2</f>
         <v>0.09855</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -1844,7 +2031,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
@@ -1986,11 +2173,11 @@
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
-      <c r="L9" s="36" t="n">
+      <c r="L9" s="42" t="n">
         <v>0.1255</v>
       </c>
       <c r="M9" s="22"/>
-      <c r="N9" s="37" t="n">
+      <c r="N9" s="43" t="n">
         <v>0.0121</v>
       </c>
       <c r="O9" s="0" t="s">
@@ -2035,11 +2222,11 @@
         <f aca="false">(0.0925+0.0919)/2</f>
         <v>0.0922</v>
       </c>
-      <c r="L10" s="38" t="n">
+      <c r="L10" s="44" t="n">
         <v>0.1578</v>
       </c>
       <c r="M10" s="16"/>
-      <c r="N10" s="39" t="n">
+      <c r="N10" s="45" t="n">
         <v>0.0837</v>
       </c>
       <c r="O10" s="0" t="s">
@@ -2054,56 +2241,56 @@
       <c r="M11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="29"/>
-      <c r="M12" s="30"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="O13" s="39" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31"/>
-      <c r="B16" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="O16" s="33" t="s">
+      <c r="A16" s="37"/>
+      <c r="B16" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="O16" s="39" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="O17" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="O17" s="39" t="s">
         <v>20</v>
       </c>
       <c r="Q17" s="0" t="s">
@@ -2111,11 +2298,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="33" t="s">
+      <c r="O18" s="39" t="s">
         <v>20</v>
       </c>
       <c r="Q18" s="0" t="s">
@@ -2123,88 +2310,88 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="38" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31"/>
-      <c r="B21" s="30" t="s">
-        <v>30</v>
+      <c r="A21" s="37"/>
+      <c r="B21" s="36" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="37" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31"/>
+      <c r="A24" s="37"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="38" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31"/>
-      <c r="B26" s="30" t="s">
-        <v>37</v>
+      <c r="A26" s="37"/>
+      <c r="B26" s="36" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="29" t="s">
-        <v>39</v>
+      <c r="B27" s="35" t="s">
+        <v>58</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="29" t="s">
-        <v>42</v>
+      <c r="B28" s="35" t="s">
+        <v>59</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="29" t="s">
-        <v>44</v>
+      <c r="B29" s="35" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>46</v>
+      <c r="A30" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2239,7 +2426,7 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F12:G13 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2249,16 +2436,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,52 +2468,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8563,7 +8750,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>0.23</v>
@@ -8587,7 +8774,7 @@
         <v>64</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -8607,7 +8794,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>0.26</v>
@@ -8637,7 +8824,7 @@
         <v>73</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -8657,7 +8844,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>0.2</v>
@@ -8687,7 +8874,7 @@
         <v>85</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -14979,17 +15166,17 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S305" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S306" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S307" s="0" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -15011,23 +15198,23 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="F12:G13 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15051,52 +15238,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21333,7 +21520,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -21351,7 +21538,7 @@
         <v>570</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -21371,7 +21558,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -21389,7 +21576,7 @@
         <v>546</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -21409,7 +21596,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -21427,7 +21614,7 @@
         <v>553</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -27719,26 +27906,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -27760,23 +27947,23 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+      <selection pane="topLeft" activeCell="T2" activeCellId="1" sqref="F12:G13 T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27800,52 +27987,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34082,7 +34269,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -34100,7 +34287,7 @@
         <v>3360</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -34120,7 +34307,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -34138,7 +34325,7 @@
         <v>3172</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -34158,7 +34345,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -34176,7 +34363,7 @@
         <v>3227</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -40468,26 +40655,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -40509,27 +40696,27 @@
   <dimension ref="A1:W307"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H303" activeCellId="0" sqref="H303"/>
+      <selection pane="topLeft" activeCell="H303" activeCellId="1" sqref="F12:G13 H303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="I1" s="0" t="n">
         <f aca="false">COUNTIF(H4:H103,"=1")</f>
         <v>72</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -40561,52 +40748,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46843,7 +47030,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -46861,7 +47048,7 @@
         <v>3281</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -46881,7 +47068,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -46899,7 +47086,7 @@
         <v>3285</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -46919,7 +47106,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -46937,7 +47124,7 @@
         <v>3161</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -53229,26 +53416,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solar table results update + deltas
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="128">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t xml:space="preserve">KNN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Best of k=[1, 50]</t>
   </si>
   <si>
     <t xml:space="preserve">Plan</t>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t xml:space="preserve">RDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best of k=[1, 50]</t>
   </si>
   <si>
     <t xml:space="preserve">Stage 1 establishes the likelihood to extract a user's dataset of transactions for stage 2</t>
@@ -420,7 +420,7 @@
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -460,6 +460,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -477,7 +484,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,12 +495,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
         <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF6F9D4"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -615,7 +616,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -712,6 +713,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -720,39 +725,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="9" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -760,7 +769,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -772,11 +781,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -784,19 +793,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="5" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -829,7 +838,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF6F9D4"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -877,10 +886,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1048576"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1138,7 +1147,7 @@
       <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="C6" s="24" t="n">
         <f aca="false">(0.429+0.4242+0.4323)/3</f>
         <v>0.4285</v>
       </c>
@@ -1214,7 +1223,7 @@
         <f aca="false">(0.6344+0.6545+0.6652)/3</f>
         <v>0.651366666666667</v>
       </c>
-      <c r="H7" s="24" t="n">
+      <c r="H7" s="25" t="n">
         <f aca="false">(0.0264+0.0266+0.0259)/3</f>
         <v>0.0263</v>
       </c>
@@ -1226,7 +1235,7 @@
         <f aca="false">(0.5855+0.5623)/2</f>
         <v>0.5739</v>
       </c>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="25" t="n">
         <f aca="false">(0.0254+0.0255)/2</f>
         <v>0.02545</v>
       </c>
@@ -1238,7 +1247,7 @@
         <f aca="false">(0.5392+0.5216)/2</f>
         <v>0.5304</v>
       </c>
-      <c r="N7" s="24" t="n">
+      <c r="N7" s="25" t="n">
         <f aca="false">(0.0269+0.0266)/2</f>
         <v>0.02675</v>
       </c>
@@ -1248,7 +1257,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="15" t="n">
@@ -1318,7 +1327,7 @@
         <f aca="false">(0.3498+0.3479+0.3496)/3</f>
         <v>0.3491</v>
       </c>
-      <c r="E9" s="24" t="n">
+      <c r="E9" s="25" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
@@ -1330,7 +1339,7 @@
         <f aca="false">(0.4779+0.4776+0.4793)/3</f>
         <v>0.478266666666667</v>
       </c>
-      <c r="H9" s="24" t="n">
+      <c r="H9" s="25" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
@@ -1342,7 +1351,7 @@
         <f aca="false">(0.5451+0.5456)/2</f>
         <v>0.54535</v>
       </c>
-      <c r="K9" s="24" t="n">
+      <c r="K9" s="25" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
@@ -1354,12 +1363,9 @@
         <f aca="false">(0.5145+0.5146)/2</f>
         <v>0.51455</v>
       </c>
-      <c r="N9" s="24" t="n">
+      <c r="N9" s="25" t="n">
         <f aca="false">(0.0239+0.0239)/2</f>
         <v>0.0239</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,16 +1421,13 @@
         <f aca="false">(0.0952+0.0952)/2</f>
         <v>0.0952</v>
       </c>
-      <c r="O10" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -1441,8 +1444,8 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
@@ -1469,8 +1472,8 @@
       <c r="H13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
@@ -1479,64 +1482,65 @@
       <c r="B14" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="28" t="n">
+      <c r="C14" s="29" t="n">
         <f aca="false">(0.6684+0.6912)/2</f>
         <v>0.6798</v>
       </c>
-      <c r="D14" s="28" t="n">
+      <c r="D14" s="29" t="n">
         <f aca="false">(0.6967+0.6607)/2</f>
         <v>0.6787</v>
       </c>
-      <c r="E14" s="28" t="n">
+      <c r="E14" s="29" t="n">
         <f aca="false">(0.0302+0.0307)/2</f>
         <v>0.03045</v>
       </c>
-      <c r="F14" s="29" t="n">
+      <c r="F14" s="30" t="n">
         <f aca="false">(0.7336)/1</f>
         <v>0.7336</v>
       </c>
-      <c r="G14" s="28" t="n">
+      <c r="G14" s="29" t="n">
         <f aca="false">(0.7158)/1</f>
         <v>0.7158</v>
       </c>
-      <c r="H14" s="30" t="n">
+      <c r="H14" s="31" t="n">
         <f aca="false">(0.0282+0.0286)/2</f>
         <v>0.0284</v>
       </c>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
+      <c r="J14" s="32"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
       <c r="B15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="31" t="n">
+      <c r="C15" s="33" t="n">
         <f aca="false">(0.5605+0.5406)/2</f>
         <v>0.55055</v>
       </c>
-      <c r="D15" s="31" t="n">
+      <c r="D15" s="33" t="n">
         <f aca="false">(0.5246+0.5207)/2</f>
         <v>0.52265</v>
       </c>
-      <c r="E15" s="31" t="n">
+      <c r="E15" s="33" t="n">
         <f aca="false">(0.1216+0.1192)/2</f>
         <v>0.1204</v>
       </c>
-      <c r="F15" s="32" t="n">
+      <c r="F15" s="34" t="n">
         <f aca="false">(0.6049)/1</f>
         <v>0.6049</v>
       </c>
-      <c r="G15" s="31" t="n">
+      <c r="G15" s="33" t="n">
         <f aca="false">(0.5747)/1</f>
         <v>0.5747</v>
       </c>
-      <c r="H15" s="33" t="n">
+      <c r="H15" s="35" t="n">
         <f aca="false">(0.1194+0.1194)/2</f>
         <v>0.1194</v>
       </c>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
@@ -1545,216 +1549,402 @@
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="29" t="n">
+      <c r="C16" s="30" t="n">
         <f aca="false">(0.7298+0.7055)/2</f>
         <v>0.71765</v>
       </c>
-      <c r="D16" s="28" t="n">
+      <c r="D16" s="29" t="n">
         <f aca="false">(0.7841+0.8337)/2</f>
         <v>0.8089</v>
       </c>
-      <c r="E16" s="30" t="n">
+      <c r="E16" s="31" t="n">
         <f aca="false">(0.0282+0.0285)/2</f>
         <v>0.02835</v>
       </c>
-      <c r="F16" s="29" t="n">
+      <c r="F16" s="30" t="n">
         <f aca="false">(0.7581+0.7598)/2</f>
         <v>0.75895</v>
       </c>
-      <c r="G16" s="28" t="n">
+      <c r="G16" s="29" t="n">
         <f aca="false">(0.7847+0.7562)/2</f>
         <v>0.77045</v>
       </c>
-      <c r="H16" s="30" t="n">
+      <c r="H16" s="31" t="n">
         <f aca="false">(0.037+0.0369)/2</f>
         <v>0.03695</v>
       </c>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="32" t="n">
+      <c r="C17" s="34" t="n">
         <f aca="false">(0.5823+0.5715)/2</f>
         <v>0.5769</v>
       </c>
-      <c r="D17" s="31" t="n">
+      <c r="D17" s="33" t="n">
         <f aca="false">(0.5692+0.5583)/2</f>
         <v>0.56375</v>
       </c>
-      <c r="E17" s="33" t="n">
+      <c r="E17" s="35" t="n">
         <f aca="false">(0.1638+0.1647)/2</f>
         <v>0.16425</v>
       </c>
-      <c r="F17" s="32" t="n">
+      <c r="F17" s="34" t="n">
         <f aca="false">(0.5205+0.5217)/2</f>
         <v>0.5211</v>
       </c>
-      <c r="G17" s="31" t="n">
+      <c r="G17" s="33" t="n">
         <f aca="false">(0.5214+0.5275)/2</f>
         <v>0.52445</v>
       </c>
-      <c r="H17" s="33" t="n">
+      <c r="H17" s="35" t="n">
         <f aca="false">(0.1307+0.1299)/2</f>
         <v>0.1303</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="s">
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="29" t="n">
+        <f aca="false">C14-C5</f>
+        <v>0.099533333333333</v>
+      </c>
+      <c r="D21" s="29" t="n">
+        <f aca="false">D14-D5</f>
+        <v>0.0866</v>
+      </c>
+      <c r="E21" s="29" t="n">
+        <f aca="false">E14-E5</f>
+        <v>0.0057833333333333</v>
+      </c>
+      <c r="F21" s="30" t="n">
+        <f aca="false">F14-F5</f>
+        <v>0.0345</v>
+      </c>
+      <c r="G21" s="29" t="n">
+        <f aca="false">G14-G5</f>
+        <v>0.00533333333333297</v>
+      </c>
+      <c r="H21" s="31" t="n">
+        <f aca="false">H14-H5</f>
+        <v>0.0045</v>
+      </c>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="19"/>
+      <c r="B22" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="33" t="n">
+        <f aca="false">C15-C6</f>
+        <v>0.12205</v>
+      </c>
+      <c r="D22" s="33" t="n">
+        <f aca="false">D15-D6</f>
+        <v>0.066183333333333</v>
+      </c>
+      <c r="E22" s="33" t="n">
+        <f aca="false">E15-E6</f>
+        <v>0.005766666666667</v>
+      </c>
+      <c r="F22" s="34" t="n">
+        <f aca="false">F15-F6</f>
+        <v>0.0652666666666669</v>
+      </c>
+      <c r="G22" s="33" t="n">
+        <f aca="false">G15-G6</f>
+        <v>0.0169666666666669</v>
+      </c>
+      <c r="H22" s="35" t="n">
+        <f aca="false">H15-H6</f>
+        <v>0.004666666666667</v>
+      </c>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="30" t="n">
+        <f aca="false">C16-C7</f>
+        <v>0.0913499999999999</v>
+      </c>
+      <c r="D23" s="29" t="n">
+        <f aca="false">D16-D7</f>
+        <v>0.160766666666667</v>
+      </c>
+      <c r="E23" s="31" t="n">
+        <f aca="false">E16-E7</f>
+        <v>0.00695</v>
+      </c>
+      <c r="F23" s="30" t="n">
+        <f aca="false">F16-F7</f>
+        <v>0.127983333333333</v>
+      </c>
+      <c r="G23" s="29" t="n">
+        <f aca="false">G16-G7</f>
+        <v>0.119083333333333</v>
+      </c>
+      <c r="H23" s="31" t="n">
+        <f aca="false">H16-H7</f>
+        <v>0.01065</v>
+      </c>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="19"/>
+      <c r="B24" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="34" t="n">
+        <f aca="false">C17-C8</f>
+        <v>0.197966666666667</v>
+      </c>
+      <c r="D24" s="33" t="n">
+        <f aca="false">D17-D8</f>
+        <v>0.156816666666667</v>
+      </c>
+      <c r="E24" s="35" t="n">
+        <f aca="false">E17-E8</f>
+        <v>0.04565</v>
+      </c>
+      <c r="F24" s="34" t="n">
+        <f aca="false">F17-F8</f>
+        <v>0.151666666666667</v>
+      </c>
+      <c r="G24" s="33" t="n">
+        <f aca="false">G17-G8</f>
+        <v>0.159216666666667</v>
+      </c>
+      <c r="H24" s="35" t="n">
+        <f aca="false">H17-H8</f>
+        <v>0.0136</v>
+      </c>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="37"/>
+      <c r="M26" s="38"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
+      <c r="B27" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="O27" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="O20" s="39" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="39" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
+      <c r="B29" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="39"/>
+      <c r="B30" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37"/>
-      <c r="B23" s="36" t="s">
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="O30" s="41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="39"/>
+      <c r="B31" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="O23" s="39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37"/>
-      <c r="B24" s="0" t="s">
+      <c r="O31" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q31" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="O24" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q24" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="39"/>
+      <c r="B32" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37"/>
-      <c r="B25" s="0" t="s">
+      <c r="O32" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O25" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q25" s="0" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="39" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
+      <c r="B34" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="38" t="s">
+    </row>
+    <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="39"/>
+      <c r="B35" s="38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="37"/>
-      <c r="B28" s="36" t="s">
+    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="39" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37" t="s">
+      <c r="B36" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="0" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="39" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
+      <c r="B37" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="0" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="39"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="39" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="37"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="37" t="s">
+      <c r="B39" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="38" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="39"/>
+      <c r="B40" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="37"/>
-      <c r="B33" s="36" t="s">
+    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="37" t="s">
+      <c r="B41" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="H41" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="0" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="39" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="37" t="s">
+      <c r="B42" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="35" t="s">
+    </row>
+    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="39" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="37" t="s">
+      <c r="B43" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="19">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
@@ -1769,6 +1959,11 @@
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A24"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1801,7 +1996,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -1825,7 +2020,7 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
@@ -1838,40 +2033,40 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="I2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="L2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
@@ -1917,7 +2112,7 @@
         <f aca="false">(0.0181+0.0175)/2</f>
         <v>0.0178</v>
       </c>
-      <c r="L3" s="40" t="n">
+      <c r="L3" s="42" t="n">
         <v>0.7585</v>
       </c>
       <c r="M3" s="12"/>
@@ -1925,11 +2120,11 @@
         <f aca="false">(0.0195+0.0186)/2</f>
         <v>0.01905</v>
       </c>
-      <c r="O3" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
+      <c r="O3" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
@@ -1978,9 +2173,9 @@
         <f aca="false">(0.0985+0.0986)/2</f>
         <v>0.09855</v>
       </c>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -2082,7 +2277,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
@@ -2107,7 +2302,7 @@
         <f aca="false">(0.2274+0.2273+0.2291)/3</f>
         <v>0.227933333333333</v>
       </c>
-      <c r="H7" s="24" t="n">
+      <c r="H7" s="25" t="n">
         <f aca="false">(0.0209+0.0207+0.0214)/3</f>
         <v>0.021</v>
       </c>
@@ -2116,7 +2311,7 @@
         <v>0.331033333333333</v>
       </c>
       <c r="J7" s="22"/>
-      <c r="K7" s="24" t="n">
+      <c r="K7" s="25" t="n">
         <f aca="false">(0.0319+0.0309+0.031)/3</f>
         <v>0.0312666666666667</v>
       </c>
@@ -2125,7 +2320,7 @@
         <v>0.3158</v>
       </c>
       <c r="M7" s="22"/>
-      <c r="N7" s="24" t="n">
+      <c r="N7" s="25" t="n">
         <f aca="false">(0.0209+0.0214)/2</f>
         <v>0.02115</v>
       </c>
@@ -2135,7 +2330,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="15" t="n">
@@ -2199,7 +2394,7 @@
         <f aca="false">(0.085+0.0874+0.0856)/3</f>
         <v>0.086</v>
       </c>
-      <c r="E9" s="24" t="n">
+      <c r="E9" s="25" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
@@ -2211,7 +2406,7 @@
         <f aca="false">(0.1109+0.1114+0.1119)/3</f>
         <v>0.1114</v>
       </c>
-      <c r="H9" s="24" t="n">
+      <c r="H9" s="25" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
@@ -2220,19 +2415,19 @@
         <v>0.1408</v>
       </c>
       <c r="J9" s="22"/>
-      <c r="K9" s="24" t="n">
+      <c r="K9" s="25" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
-      <c r="L9" s="42" t="n">
+      <c r="L9" s="44" t="n">
         <v>0.1255</v>
       </c>
       <c r="M9" s="22"/>
-      <c r="N9" s="43" t="n">
+      <c r="N9" s="45" t="n">
         <v>0.0121</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,175 +2468,175 @@
         <f aca="false">(0.0925+0.0919)/2</f>
         <v>0.0922</v>
       </c>
-      <c r="L10" s="44" t="n">
+      <c r="L10" s="46" t="n">
         <v>0.1578</v>
       </c>
       <c r="M10" s="16"/>
-      <c r="N10" s="45" t="n">
+      <c r="N10" s="47" t="n">
         <v>0.0837</v>
       </c>
       <c r="O10" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="s">
+      <c r="L12" s="37"/>
+      <c r="M12" s="38"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="35"/>
-      <c r="M12" s="36"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
+      <c r="B13" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="O13" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="O13" s="39" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="39" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
+      <c r="B15" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37"/>
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="O16" s="39" t="s">
-        <v>20</v>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="O16" s="41" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="O17" s="39" t="s">
-        <v>20</v>
+      <c r="O17" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="Q17" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="39"/>
+      <c r="B18" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37"/>
-      <c r="B18" s="0" t="s">
+      <c r="O18" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="O18" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q18" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="39" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="37" t="s">
+      <c r="B20" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="37"/>
-      <c r="B21" s="36" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="38" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
-        <v>31</v>
+      <c r="A22" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37" t="s">
-        <v>33</v>
+      <c r="A23" s="39" t="s">
+        <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="37"/>
+      <c r="A24" s="39"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="38" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="37"/>
-      <c r="B26" s="36" t="s">
+      <c r="A26" s="39"/>
+      <c r="B26" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="35" t="s">
+      <c r="A27" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="37" t="s">
         <v>58</v>
       </c>
       <c r="H27" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="39" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="37" t="s">
         <v>59</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="35" t="s">
+      <c r="A29" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="37" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="37" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Obj 3 classification graphs produced
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -420,7 +420,7 @@
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -457,13 +457,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
       <charset val="1"/>
     </font>
     <font>
@@ -616,7 +609,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -713,10 +706,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -725,23 +714,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -749,19 +726,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -769,7 +734,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -889,7 +854,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1147,7 +1112,7 @@
       <c r="B6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="24" t="n">
+      <c r="C6" s="21" t="n">
         <f aca="false">(0.429+0.4242+0.4323)/3</f>
         <v>0.4285</v>
       </c>
@@ -1223,7 +1188,7 @@
         <f aca="false">(0.6344+0.6545+0.6652)/3</f>
         <v>0.651366666666667</v>
       </c>
-      <c r="H7" s="25" t="n">
+      <c r="H7" s="24" t="n">
         <f aca="false">(0.0264+0.0266+0.0259)/3</f>
         <v>0.0263</v>
       </c>
@@ -1235,7 +1200,7 @@
         <f aca="false">(0.5855+0.5623)/2</f>
         <v>0.5739</v>
       </c>
-      <c r="K7" s="25" t="n">
+      <c r="K7" s="24" t="n">
         <f aca="false">(0.0254+0.0255)/2</f>
         <v>0.02545</v>
       </c>
@@ -1247,7 +1212,7 @@
         <f aca="false">(0.5392+0.5216)/2</f>
         <v>0.5304</v>
       </c>
-      <c r="N7" s="25" t="n">
+      <c r="N7" s="24" t="n">
         <f aca="false">(0.0269+0.0266)/2</f>
         <v>0.02675</v>
       </c>
@@ -1257,7 +1222,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="15" t="n">
@@ -1327,7 +1292,7 @@
         <f aca="false">(0.3498+0.3479+0.3496)/3</f>
         <v>0.3491</v>
       </c>
-      <c r="E9" s="25" t="n">
+      <c r="E9" s="24" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
@@ -1339,7 +1304,7 @@
         <f aca="false">(0.4779+0.4776+0.4793)/3</f>
         <v>0.478266666666667</v>
       </c>
-      <c r="H9" s="25" t="n">
+      <c r="H9" s="24" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
@@ -1351,7 +1316,7 @@
         <f aca="false">(0.5451+0.5456)/2</f>
         <v>0.54535</v>
       </c>
-      <c r="K9" s="25" t="n">
+      <c r="K9" s="24" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
@@ -1363,7 +1328,7 @@
         <f aca="false">(0.5145+0.5146)/2</f>
         <v>0.51455</v>
       </c>
-      <c r="N9" s="25" t="n">
+      <c r="N9" s="24" t="n">
         <f aca="false">(0.0239+0.0239)/2</f>
         <v>0.0239</v>
       </c>
@@ -1423,11 +1388,11 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -1444,8 +1409,8 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
@@ -1472,8 +1437,8 @@
       <c r="H13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
@@ -1482,65 +1447,65 @@
       <c r="B14" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="29" t="n">
+      <c r="C14" s="12" t="n">
         <f aca="false">(0.6684+0.6912)/2</f>
         <v>0.6798</v>
       </c>
-      <c r="D14" s="29" t="n">
+      <c r="D14" s="12" t="n">
         <f aca="false">(0.6967+0.6607)/2</f>
         <v>0.6787</v>
       </c>
-      <c r="E14" s="29" t="n">
+      <c r="E14" s="12" t="n">
         <f aca="false">(0.0302+0.0307)/2</f>
         <v>0.03045</v>
       </c>
-      <c r="F14" s="30" t="n">
-        <f aca="false">(0.7336)/1</f>
-        <v>0.7336</v>
-      </c>
-      <c r="G14" s="29" t="n">
-        <f aca="false">(0.7158)/1</f>
-        <v>0.7158</v>
-      </c>
-      <c r="H14" s="31" t="n">
+      <c r="F14" s="11" t="n">
+        <f aca="false">(0.7636)/1</f>
+        <v>0.7636</v>
+      </c>
+      <c r="G14" s="12" t="n">
+        <f aca="false">(0.7658)/1</f>
+        <v>0.7658</v>
+      </c>
+      <c r="H14" s="13" t="n">
         <f aca="false">(0.0282+0.0286)/2</f>
         <v>0.0284</v>
       </c>
-      <c r="J14" s="32"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
       <c r="B15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="33" t="n">
+      <c r="C15" s="16" t="n">
         <f aca="false">(0.5605+0.5406)/2</f>
         <v>0.55055</v>
       </c>
-      <c r="D15" s="33" t="n">
+      <c r="D15" s="16" t="n">
         <f aca="false">(0.5246+0.5207)/2</f>
         <v>0.52265</v>
       </c>
-      <c r="E15" s="33" t="n">
+      <c r="E15" s="16" t="n">
         <f aca="false">(0.1216+0.1192)/2</f>
         <v>0.1204</v>
       </c>
-      <c r="F15" s="34" t="n">
-        <f aca="false">(0.6049)/1</f>
-        <v>0.6049</v>
-      </c>
-      <c r="G15" s="33" t="n">
-        <f aca="false">(0.5747)/1</f>
-        <v>0.5747</v>
-      </c>
-      <c r="H15" s="35" t="n">
+      <c r="F15" s="15" t="n">
+        <f aca="false">(0.6249)/1</f>
+        <v>0.6249</v>
+      </c>
+      <c r="G15" s="16" t="n">
+        <f aca="false">(0.5947)/1</f>
+        <v>0.5947</v>
+      </c>
+      <c r="H15" s="17" t="n">
         <f aca="false">(0.1194+0.1194)/2</f>
         <v>0.1194</v>
       </c>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
@@ -1549,68 +1514,68 @@
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="30" t="n">
+      <c r="C16" s="11" t="n">
         <f aca="false">(0.7298+0.7055)/2</f>
         <v>0.71765</v>
       </c>
-      <c r="D16" s="29" t="n">
-        <f aca="false">(0.7841+0.8337)/2</f>
-        <v>0.8089</v>
-      </c>
-      <c r="E16" s="31" t="n">
+      <c r="D16" s="12" t="n">
+        <f aca="false">(0.7541+0.7637)/2</f>
+        <v>0.7589</v>
+      </c>
+      <c r="E16" s="13" t="n">
         <f aca="false">(0.0282+0.0285)/2</f>
         <v>0.02835</v>
       </c>
-      <c r="F16" s="30" t="n">
-        <f aca="false">(0.7581+0.7598)/2</f>
-        <v>0.75895</v>
-      </c>
-      <c r="G16" s="29" t="n">
-        <f aca="false">(0.7847+0.7562)/2</f>
-        <v>0.77045</v>
-      </c>
-      <c r="H16" s="31" t="n">
+      <c r="F16" s="11" t="n">
+        <f aca="false">(0.7281+0.7298)/2</f>
+        <v>0.72895</v>
+      </c>
+      <c r="G16" s="12" t="n">
+        <f aca="false">(0.7447+0.7462)/2</f>
+        <v>0.74545</v>
+      </c>
+      <c r="H16" s="13" t="n">
         <f aca="false">(0.037+0.0369)/2</f>
         <v>0.03695</v>
       </c>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="34" t="n">
+      <c r="C17" s="15" t="n">
         <f aca="false">(0.5823+0.5715)/2</f>
         <v>0.5769</v>
       </c>
-      <c r="D17" s="33" t="n">
-        <f aca="false">(0.5692+0.5583)/2</f>
-        <v>0.56375</v>
-      </c>
-      <c r="E17" s="35" t="n">
-        <f aca="false">(0.1638+0.1647)/2</f>
-        <v>0.16425</v>
-      </c>
-      <c r="F17" s="34" t="n">
+      <c r="D17" s="16" t="n">
+        <f aca="false">(0.5892+0.5783)/2</f>
+        <v>0.58375</v>
+      </c>
+      <c r="E17" s="17" t="n">
+        <f aca="false">(0.1438+0.1447)/2</f>
+        <v>0.14425</v>
+      </c>
+      <c r="F17" s="15" t="n">
         <f aca="false">(0.5205+0.5217)/2</f>
         <v>0.5211</v>
       </c>
-      <c r="G17" s="33" t="n">
+      <c r="G17" s="16" t="n">
         <f aca="false">(0.5214+0.5275)/2</f>
         <v>0.52445</v>
       </c>
-      <c r="H17" s="35" t="n">
+      <c r="H17" s="17" t="n">
         <f aca="false">(0.1307+0.1299)/2</f>
         <v>0.1303</v>
       </c>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -1627,8 +1592,8 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
@@ -1655,8 +1620,8 @@
       <c r="H20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
@@ -1665,64 +1630,64 @@
       <c r="B21" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="29" t="n">
+      <c r="C21" s="12" t="n">
         <f aca="false">C14-C5</f>
         <v>0.099533333333333</v>
       </c>
-      <c r="D21" s="29" t="n">
+      <c r="D21" s="12" t="n">
         <f aca="false">D14-D5</f>
         <v>0.0866</v>
       </c>
-      <c r="E21" s="29" t="n">
+      <c r="E21" s="12" t="n">
         <f aca="false">E14-E5</f>
         <v>0.0057833333333333</v>
       </c>
-      <c r="F21" s="30" t="n">
+      <c r="F21" s="11" t="n">
         <f aca="false">F14-F5</f>
-        <v>0.0345</v>
-      </c>
-      <c r="G21" s="29" t="n">
+        <v>0.0645</v>
+      </c>
+      <c r="G21" s="12" t="n">
         <f aca="false">G14-G5</f>
-        <v>0.00533333333333297</v>
-      </c>
-      <c r="H21" s="31" t="n">
+        <v>0.055333333333333</v>
+      </c>
+      <c r="H21" s="13" t="n">
         <f aca="false">H14-H5</f>
         <v>0.0045</v>
       </c>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
       <c r="B22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="33" t="n">
+      <c r="C22" s="16" t="n">
         <f aca="false">C15-C6</f>
         <v>0.12205</v>
       </c>
-      <c r="D22" s="33" t="n">
+      <c r="D22" s="16" t="n">
         <f aca="false">D15-D6</f>
         <v>0.066183333333333</v>
       </c>
-      <c r="E22" s="33" t="n">
+      <c r="E22" s="16" t="n">
         <f aca="false">E15-E6</f>
         <v>0.005766666666667</v>
       </c>
-      <c r="F22" s="34" t="n">
+      <c r="F22" s="15" t="n">
         <f aca="false">F15-F6</f>
-        <v>0.0652666666666669</v>
-      </c>
-      <c r="G22" s="33" t="n">
+        <v>0.0852666666666669</v>
+      </c>
+      <c r="G22" s="16" t="n">
         <f aca="false">G15-G6</f>
-        <v>0.0169666666666669</v>
-      </c>
-      <c r="H22" s="35" t="n">
+        <v>0.0369666666666669</v>
+      </c>
+      <c r="H22" s="17" t="n">
         <f aca="false">H15-H6</f>
         <v>0.004666666666667</v>
       </c>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
@@ -1731,126 +1696,126 @@
       <c r="B23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="30" t="n">
+      <c r="C23" s="11" t="n">
         <f aca="false">C16-C7</f>
         <v>0.0913499999999999</v>
       </c>
-      <c r="D23" s="29" t="n">
+      <c r="D23" s="12" t="n">
         <f aca="false">D16-D7</f>
-        <v>0.160766666666667</v>
-      </c>
-      <c r="E23" s="31" t="n">
+        <v>0.110766666666667</v>
+      </c>
+      <c r="E23" s="13" t="n">
         <f aca="false">E16-E7</f>
         <v>0.00695</v>
       </c>
-      <c r="F23" s="30" t="n">
+      <c r="F23" s="11" t="n">
         <f aca="false">F16-F7</f>
-        <v>0.127983333333333</v>
-      </c>
-      <c r="G23" s="29" t="n">
+        <v>0.097983333333333</v>
+      </c>
+      <c r="G23" s="12" t="n">
         <f aca="false">G16-G7</f>
-        <v>0.119083333333333</v>
-      </c>
-      <c r="H23" s="31" t="n">
+        <v>0.094083333333333</v>
+      </c>
+      <c r="H23" s="13" t="n">
         <f aca="false">H16-H7</f>
         <v>0.01065</v>
       </c>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="34" t="n">
+      <c r="C24" s="15" t="n">
         <f aca="false">C17-C8</f>
         <v>0.197966666666667</v>
       </c>
-      <c r="D24" s="33" t="n">
+      <c r="D24" s="16" t="n">
         <f aca="false">D17-D8</f>
-        <v>0.156816666666667</v>
-      </c>
-      <c r="E24" s="35" t="n">
+        <v>0.176816666666667</v>
+      </c>
+      <c r="E24" s="17" t="n">
         <f aca="false">E17-E8</f>
-        <v>0.04565</v>
-      </c>
-      <c r="F24" s="34" t="n">
+        <v>0.02565</v>
+      </c>
+      <c r="F24" s="15" t="n">
         <f aca="false">F17-F8</f>
         <v>0.151666666666667</v>
       </c>
-      <c r="G24" s="33" t="n">
+      <c r="G24" s="16" t="n">
         <f aca="false">G17-G8</f>
         <v>0.159216666666667</v>
       </c>
-      <c r="H24" s="35" t="n">
+      <c r="H24" s="17" t="n">
         <f aca="false">H17-H8</f>
         <v>0.0136</v>
       </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L26" s="37"/>
-      <c r="M26" s="38"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="31"/>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="O27" s="41" t="s">
+      <c r="O27" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="39"/>
-      <c r="B30" s="38" t="s">
+      <c r="A30" s="32"/>
+      <c r="B30" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
-      <c r="O30" s="41" t="s">
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="O30" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="39"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="O31" s="41" t="s">
+      <c r="O31" s="34" t="s">
         <v>19</v>
       </c>
       <c r="Q31" s="0" t="s">
@@ -1858,11 +1823,11 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="39"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="O32" s="41" t="s">
+      <c r="O32" s="34" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="0" t="s">
@@ -1870,21 +1835,21 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="39" t="s">
+      <c r="A34" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="33" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="39"/>
-      <c r="B35" s="38" t="s">
+      <c r="A35" s="32"/>
+      <c r="B35" s="31" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="0" t="s">
@@ -1892,7 +1857,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="32" t="s">
         <v>32</v>
       </c>
       <c r="B37" s="0" t="s">
@@ -1900,27 +1865,27 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="39"/>
+      <c r="A38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="39"/>
-      <c r="B40" s="38" t="s">
+      <c r="A40" s="32"/>
+      <c r="B40" s="31" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="30" t="s">
         <v>38</v>
       </c>
       <c r="H41" s="0" t="s">
@@ -1928,18 +1893,18 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="30" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2112,7 +2077,7 @@
         <f aca="false">(0.0181+0.0175)/2</f>
         <v>0.0178</v>
       </c>
-      <c r="L3" s="42" t="n">
+      <c r="L3" s="35" t="n">
         <v>0.7585</v>
       </c>
       <c r="M3" s="12"/>
@@ -2120,11 +2085,11 @@
         <f aca="false">(0.0195+0.0186)/2</f>
         <v>0.01905</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
@@ -2173,9 +2138,9 @@
         <f aca="false">(0.0985+0.0986)/2</f>
         <v>0.09855</v>
       </c>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
@@ -2302,7 +2267,7 @@
         <f aca="false">(0.2274+0.2273+0.2291)/3</f>
         <v>0.227933333333333</v>
       </c>
-      <c r="H7" s="25" t="n">
+      <c r="H7" s="24" t="n">
         <f aca="false">(0.0209+0.0207+0.0214)/3</f>
         <v>0.021</v>
       </c>
@@ -2311,7 +2276,7 @@
         <v>0.331033333333333</v>
       </c>
       <c r="J7" s="22"/>
-      <c r="K7" s="25" t="n">
+      <c r="K7" s="24" t="n">
         <f aca="false">(0.0319+0.0309+0.031)/3</f>
         <v>0.0312666666666667</v>
       </c>
@@ -2320,7 +2285,7 @@
         <v>0.3158</v>
       </c>
       <c r="M7" s="22"/>
-      <c r="N7" s="25" t="n">
+      <c r="N7" s="24" t="n">
         <f aca="false">(0.0209+0.0214)/2</f>
         <v>0.02115</v>
       </c>
@@ -2330,7 +2295,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="15" t="n">
@@ -2394,7 +2359,7 @@
         <f aca="false">(0.085+0.0874+0.0856)/3</f>
         <v>0.086</v>
       </c>
-      <c r="E9" s="25" t="n">
+      <c r="E9" s="24" t="n">
         <f aca="false">(0.0097+0.0095+0.0093)/3</f>
         <v>0.0095</v>
       </c>
@@ -2406,7 +2371,7 @@
         <f aca="false">(0.1109+0.1114+0.1119)/3</f>
         <v>0.1114</v>
       </c>
-      <c r="H9" s="25" t="n">
+      <c r="H9" s="24" t="n">
         <f aca="false">(0.0187+0.0184+0.0187)/3</f>
         <v>0.0186</v>
       </c>
@@ -2415,15 +2380,15 @@
         <v>0.1408</v>
       </c>
       <c r="J9" s="22"/>
-      <c r="K9" s="25" t="n">
+      <c r="K9" s="24" t="n">
         <f aca="false">(0.0221+0.0222)/2</f>
         <v>0.02215</v>
       </c>
-      <c r="L9" s="44" t="n">
+      <c r="L9" s="37" t="n">
         <v>0.1255</v>
       </c>
       <c r="M9" s="22"/>
-      <c r="N9" s="45" t="n">
+      <c r="N9" s="38" t="n">
         <v>0.0121</v>
       </c>
       <c r="O9" s="0" t="s">
@@ -2468,11 +2433,11 @@
         <f aca="false">(0.0925+0.0919)/2</f>
         <v>0.0922</v>
       </c>
-      <c r="L10" s="46" t="n">
+      <c r="L10" s="39" t="n">
         <v>0.1578</v>
       </c>
       <c r="M10" s="16"/>
-      <c r="N10" s="47" t="n">
+      <c r="N10" s="40" t="n">
         <v>0.0837</v>
       </c>
       <c r="O10" s="0" t="s">
@@ -2480,63 +2445,63 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L12" s="37"/>
-      <c r="M12" s="38"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="41" t="s">
+      <c r="O13" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39"/>
-      <c r="B16" s="38" t="s">
+      <c r="A16" s="32"/>
+      <c r="B16" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="O16" s="41" t="s">
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="O16" s="34" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="O17" s="41" t="s">
+      <c r="O17" s="34" t="s">
         <v>19</v>
       </c>
       <c r="Q17" s="0" t="s">
@@ -2544,11 +2509,11 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="O18" s="41" t="s">
+      <c r="O18" s="34" t="s">
         <v>19</v>
       </c>
       <c r="Q18" s="0" t="s">
@@ -2556,21 +2521,21 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="33" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="39"/>
-      <c r="B21" s="38" t="s">
+      <c r="A21" s="32"/>
+      <c r="B21" s="31" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="32" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="0" t="s">
@@ -2578,7 +2543,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="32" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="0" t="s">
@@ -2586,27 +2551,27 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="39"/>
+      <c r="A24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="33" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39"/>
-      <c r="B26" s="38" t="s">
+      <c r="A26" s="32"/>
+      <c r="B26" s="31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="30" t="s">
         <v>58</v>
       </c>
       <c r="H27" s="0" t="s">
@@ -2614,10 +2579,10 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="30" t="s">
         <v>59</v>
       </c>
       <c r="H28" s="0" t="s">
@@ -2625,18 +2590,18 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="30" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Results and graphs for rfc hourly with solar
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="116">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">KNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELTA</t>
   </si>
   <si>
     <t xml:space="preserve">Plan</t>
@@ -821,6 +824,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1141,11 +1145,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="55332178"/>
-        <c:axId val="10970441"/>
+        <c:axId val="18701851"/>
+        <c:axId val="97005762"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55332178"/>
+        <c:axId val="18701851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1201,7 +1205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10970441"/>
+        <c:crossAx val="97005762"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1209,7 +1213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10970441"/>
+        <c:axId val="97005762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1256,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1274,7 +1278,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55332178"/>
+        <c:crossAx val="18701851"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1294,7 +1298,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -1312,9 +1316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>806400</xdr:colOff>
+      <xdr:colOff>805680</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1323,7 +1327,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5249880" y="9319320"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1343,8 +1347,8 @@
   </sheetPr>
   <dimension ref="A1:Q316"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1899,6 +1903,11 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="27"/>
       <c r="M12" s="27"/>
     </row>
@@ -1927,6 +1936,15 @@
       <c r="H13" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="I13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
     </row>
@@ -1961,7 +1979,9 @@
         <f aca="false">(0.0282+0.0286)/2</f>
         <v>0.0284</v>
       </c>
-      <c r="J14" s="28"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
@@ -1994,6 +2014,9 @@
         <f aca="false">(0.1194+0.1194)/2</f>
         <v>0.1194</v>
       </c>
+      <c r="I15" s="15"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
     </row>
@@ -2027,6 +2050,15 @@
       <c r="H16" s="13" t="n">
         <f aca="false">(0.037+0.0369)/2</f>
         <v>0.03695</v>
+      </c>
+      <c r="I16" s="21" t="n">
+        <v>0.7456</v>
+      </c>
+      <c r="J16" s="22" t="n">
+        <v>0.7261</v>
+      </c>
+      <c r="K16" s="24" t="n">
+        <v>0.0508</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
@@ -2060,6 +2092,15 @@
         <f aca="false">(0.1307+0.1299)/2</f>
         <v>0.1303</v>
       </c>
+      <c r="I17" s="15" t="n">
+        <v>0.479</v>
+      </c>
+      <c r="J17" s="16" t="n">
+        <v>0.4777</v>
+      </c>
+      <c r="K17" s="17" t="n">
+        <v>0.1255</v>
+      </c>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
     </row>
@@ -2069,7 +2110,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
@@ -2082,6 +2123,11 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
       <c r="L19" s="27"/>
       <c r="M19" s="27"/>
     </row>
@@ -2110,6 +2156,15 @@
       <c r="H20" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="I20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
     </row>
@@ -2143,6 +2198,18 @@
       <c r="H21" s="13" t="n">
         <f aca="false">H14-H5</f>
         <v>0.0045</v>
+      </c>
+      <c r="I21" s="11" t="n">
+        <f aca="false">I14-I5</f>
+        <v>-0.78915</v>
+      </c>
+      <c r="J21" s="12" t="n">
+        <f aca="false">J14-J5</f>
+        <v>-0.79395</v>
+      </c>
+      <c r="K21" s="13" t="n">
+        <f aca="false">K14-K5</f>
+        <v>-0.0233</v>
       </c>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
@@ -2176,6 +2243,18 @@
         <f aca="false">H15-H6</f>
         <v>0.00466666666666667</v>
       </c>
+      <c r="I22" s="15" t="n">
+        <f aca="false">I15-I6</f>
+        <v>-0.6184</v>
+      </c>
+      <c r="J22" s="16" t="n">
+        <f aca="false">J15-J6</f>
+        <v>-0.62785</v>
+      </c>
+      <c r="K22" s="17" t="n">
+        <f aca="false">K15-K6</f>
+        <v>-0.10115</v>
+      </c>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
     </row>
@@ -2209,6 +2288,18 @@
       <c r="H23" s="13" t="n">
         <f aca="false">H16-H7</f>
         <v>0.01065</v>
+      </c>
+      <c r="I23" s="11" t="n">
+        <f aca="false">I16-I7</f>
+        <v>0.17825</v>
+      </c>
+      <c r="J23" s="12" t="n">
+        <f aca="false">J16-J7</f>
+        <v>0.1522</v>
+      </c>
+      <c r="K23" s="13" t="n">
+        <f aca="false">K16-K7</f>
+        <v>0.02535</v>
       </c>
       <c r="L23" s="27"/>
       <c r="M23" s="27"/>
@@ -2241,6 +2332,18 @@
       <c r="H24" s="17" t="n">
         <f aca="false">H17-H8</f>
         <v>0.0136</v>
+      </c>
+      <c r="I24" s="15" t="n">
+        <f aca="false">I17-I8</f>
+        <v>0.14805</v>
+      </c>
+      <c r="J24" s="16" t="n">
+        <f aca="false">J17-J8</f>
+        <v>0.1454</v>
+      </c>
+      <c r="K24" s="17" t="n">
+        <f aca="false">K17-K8</f>
+        <v>0.0212</v>
       </c>
       <c r="L24" s="27"/>
       <c r="M24" s="27"/>
@@ -2257,29 +2360,29 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L26" s="30"/>
       <c r="M26" s="31"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L27" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
@@ -2289,77 +2392,77 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="32"/>
       <c r="B30" s="31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
       <c r="K30" s="33"/>
       <c r="L30" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M30" s="33"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="32"/>
       <c r="B31" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L31" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q31" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="32"/>
       <c r="B32" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L32" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q32" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="32"/>
       <c r="B35" s="31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L35" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L36" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L37" s="34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,65 +2470,65 @@
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="32"/>
       <c r="B40" s="31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2436,7 +2539,7 @@
         <v>91</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E47" s="0" t="n">
         <f aca="false">AVERAGE(A47:A316)</f>
@@ -2467,7 +2570,7 @@
         <v>10</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E48" s="0" t="n">
         <f aca="false">AVERAGE(B47:B316)</f>
@@ -6407,7 +6510,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
@@ -6420,11 +6523,13 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:K12"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
   </mergeCells>
@@ -6446,7 +6551,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6457,16 +6562,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6489,52 +6594,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12771,7 +12876,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>0.23</v>
@@ -12795,7 +12900,7 @@
         <v>64</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -12815,7 +12920,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>0.26</v>
@@ -12845,7 +12950,7 @@
         <v>73</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -12865,7 +12970,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>0.2</v>
@@ -12895,7 +13000,7 @@
         <v>85</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -19187,17 +19292,17 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S305" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S306" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S307" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -19218,7 +19323,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -19226,16 +19331,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19259,52 +19364,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25541,7 +25646,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -25559,7 +25664,7 @@
         <v>570</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -25579,7 +25684,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -25597,7 +25702,7 @@
         <v>546</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -25617,7 +25722,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -25635,7 +25740,7 @@
         <v>553</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -31927,26 +32032,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -31967,7 +32072,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
@@ -31975,16 +32080,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32008,52 +32113,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38290,7 +38395,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -38308,7 +38413,7 @@
         <v>3360</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -38328,7 +38433,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -38346,7 +38451,7 @@
         <v>3172</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -38366,7 +38471,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -38384,7 +38489,7 @@
         <v>3227</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -44676,26 +44781,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -44716,7 +44821,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H303" activeCellId="0" sqref="H303"/>
     </sheetView>
   </sheetViews>
@@ -44724,20 +44829,20 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="0" t="n">
         <f aca="false">COUNTIF(H4:H103,"=1")</f>
         <v>72</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44769,52 +44874,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="0" t="s">
+      <c r="K3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="O3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="P3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="U3" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="V3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="W3" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51051,7 +51156,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -51069,7 +51174,7 @@
         <v>3281</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -51089,7 +51194,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -51107,7 +51212,7 @@
         <v>3285</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -51127,7 +51232,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -51145,7 +51250,7 @@
         <v>3161</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -57437,26 +57542,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remainder of CNN results for solar hourly
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -789,7 +789,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1145,11 +1145,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="18701851"/>
-        <c:axId val="97005762"/>
+        <c:axId val="80438760"/>
+        <c:axId val="7501312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18701851"/>
+        <c:axId val="80438760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97005762"/>
+        <c:crossAx val="7501312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1213,7 +1213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97005762"/>
+        <c:axId val="7501312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1278,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18701851"/>
+        <c:crossAx val="80438760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1316,9 +1316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>805680</xdr:colOff>
+      <xdr:colOff>804240</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>173880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1327,7 +1327,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5249880" y="9319320"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:ext cx="5757480" cy="3237480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:Q316"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1979,9 +1979,15 @@
         <f aca="false">(0.0282+0.0286)/2</f>
         <v>0.0284</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
+      <c r="I14" s="11" t="n">
+        <v>0.8233</v>
+      </c>
+      <c r="J14" s="12" t="n">
+        <v>0.8349</v>
+      </c>
+      <c r="K14" s="13" t="n">
+        <v>0.0331</v>
+      </c>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
@@ -2014,9 +2020,15 @@
         <f aca="false">(0.1194+0.1194)/2</f>
         <v>0.1194</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
+      <c r="I15" s="15" t="n">
+        <v>0.6614</v>
+      </c>
+      <c r="J15" s="16" t="n">
+        <v>0.6506</v>
+      </c>
+      <c r="K15" s="17" t="n">
+        <v>0.1055</v>
+      </c>
       <c r="L15" s="27"/>
       <c r="M15" s="27"/>
     </row>
@@ -2052,10 +2064,10 @@
         <v>0.03695</v>
       </c>
       <c r="I16" s="21" t="n">
-        <v>0.7456</v>
+        <v>0.7056</v>
       </c>
       <c r="J16" s="22" t="n">
-        <v>0.7261</v>
+        <v>0.7161</v>
       </c>
       <c r="K16" s="24" t="n">
         <v>0.0508</v>
@@ -2201,15 +2213,15 @@
       </c>
       <c r="I21" s="11" t="n">
         <f aca="false">I14-I5</f>
-        <v>-0.78915</v>
+        <v>0.03415</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">J14-J5</f>
-        <v>-0.79395</v>
+        <v>0.0409499999999999</v>
       </c>
       <c r="K21" s="13" t="n">
         <f aca="false">K14-K5</f>
-        <v>-0.0233</v>
+        <v>0.0098</v>
       </c>
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
@@ -2245,15 +2257,15 @@
       </c>
       <c r="I22" s="15" t="n">
         <f aca="false">I15-I6</f>
-        <v>-0.6184</v>
+        <v>0.0429999999999999</v>
       </c>
       <c r="J22" s="16" t="n">
         <f aca="false">J15-J6</f>
-        <v>-0.62785</v>
+        <v>0.02275</v>
       </c>
       <c r="K22" s="17" t="n">
         <f aca="false">K15-K6</f>
-        <v>-0.10115</v>
+        <v>0.00435000000000001</v>
       </c>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
@@ -2291,11 +2303,11 @@
       </c>
       <c r="I23" s="11" t="n">
         <f aca="false">I16-I7</f>
-        <v>0.17825</v>
+        <v>0.13825</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">J16-J7</f>
-        <v>0.1522</v>
+        <v>0.1422</v>
       </c>
       <c r="K23" s="13" t="n">
         <f aca="false">K16-K7</f>

</xml_diff>

<commit_message>
Results for half hourly solar
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -1145,11 +1145,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="80438760"/>
-        <c:axId val="7501312"/>
+        <c:axId val="75475290"/>
+        <c:axId val="49332515"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80438760"/>
+        <c:axId val="75475290"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7501312"/>
+        <c:crossAx val="49332515"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1213,7 +1213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7501312"/>
+        <c:axId val="49332515"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1278,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80438760"/>
+        <c:crossAx val="75475290"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1312,13 +1312,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>87480</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>804240</xdr:colOff>
+      <xdr:colOff>801720</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>171720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1326,8 +1326,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5249880" y="9319320"/>
-        <a:ext cx="5757480" cy="3237480"/>
+        <a:off x="5249880" y="9319680"/>
+        <a:ext cx="5754960" cy="3234960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:Q316"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1703,8 +1703,8 @@
         <v>0.5698</v>
       </c>
       <c r="M7" s="22" t="n">
-        <f aca="false">(0.5392+0.5216)/2</f>
-        <v>0.5304</v>
+        <f aca="false">(0.5692+0.5616)/2</f>
+        <v>0.5654</v>
       </c>
       <c r="N7" s="24" t="n">
         <f aca="false">(0.0269+0.0266)/2</f>
@@ -1908,8 +1908,11 @@
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
+      <c r="L12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
@@ -1945,8 +1948,15 @@
       <c r="K13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
+      <c r="L13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="19" t="s">
@@ -1988,8 +1998,15 @@
       <c r="K14" s="13" t="n">
         <v>0.0331</v>
       </c>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
+      <c r="L14" s="11" t="n">
+        <v>0.8181</v>
+      </c>
+      <c r="M14" s="12" t="n">
+        <v>0.8268</v>
+      </c>
+      <c r="N14" s="13" t="n">
+        <v>0.035</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="19"/>
@@ -2029,8 +2046,15 @@
       <c r="K15" s="17" t="n">
         <v>0.1055</v>
       </c>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
+      <c r="L15" s="15" t="n">
+        <v>0.6485</v>
+      </c>
+      <c r="M15" s="16" t="n">
+        <v>0.6698</v>
+      </c>
+      <c r="N15" s="17" t="n">
+        <v>0.1057</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="19" t="s">
@@ -2064,16 +2088,23 @@
         <v>0.03695</v>
       </c>
       <c r="I16" s="21" t="n">
-        <v>0.7056</v>
+        <v>0.6656</v>
       </c>
       <c r="J16" s="22" t="n">
-        <v>0.7161</v>
+        <v>0.6761</v>
       </c>
       <c r="K16" s="24" t="n">
         <v>0.0508</v>
       </c>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
+      <c r="L16" s="21" t="n">
+        <v>0.6762</v>
+      </c>
+      <c r="M16" s="22" t="n">
+        <v>0.6881</v>
+      </c>
+      <c r="N16" s="24" t="n">
+        <v>0.0517</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="19"/>
@@ -2113,8 +2144,15 @@
       <c r="K17" s="17" t="n">
         <v>0.1255</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
+      <c r="L17" s="15" t="n">
+        <v>0.4852</v>
+      </c>
+      <c r="M17" s="16" t="n">
+        <v>0.4851</v>
+      </c>
+      <c r="N17" s="17" t="n">
+        <v>0.1148</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L18" s="27"/>
@@ -2140,8 +2178,11 @@
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
+      <c r="L19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
@@ -2177,8 +2218,15 @@
       <c r="K20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
+      <c r="L20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
@@ -2223,8 +2271,18 @@
         <f aca="false">K14-K5</f>
         <v>0.0098</v>
       </c>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
+      <c r="L21" s="11" t="n">
+        <f aca="false">L14-L5</f>
+        <v>-0.0216500000000001</v>
+      </c>
+      <c r="M21" s="12" t="n">
+        <f aca="false">M14-M5</f>
+        <v>-0.0253</v>
+      </c>
+      <c r="N21" s="13" t="n">
+        <f aca="false">N14-N5</f>
+        <v>0.0102</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
@@ -2267,8 +2325,18 @@
         <f aca="false">K15-K6</f>
         <v>0.00435000000000001</v>
       </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
+      <c r="L22" s="15" t="n">
+        <f aca="false">L15-L6</f>
+        <v>0.0307499999999999</v>
+      </c>
+      <c r="M22" s="16" t="n">
+        <f aca="false">M15-M6</f>
+        <v>0.0354</v>
+      </c>
+      <c r="N22" s="17" t="n">
+        <f aca="false">N15-N6</f>
+        <v>0.0054</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
@@ -2303,18 +2371,28 @@
       </c>
       <c r="I23" s="11" t="n">
         <f aca="false">I16-I7</f>
-        <v>0.13825</v>
+        <v>0.0982499999999999</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">J16-J7</f>
-        <v>0.1422</v>
+        <v>0.1022</v>
       </c>
       <c r="K23" s="13" t="n">
         <f aca="false">K16-K7</f>
         <v>0.02535</v>
       </c>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
+      <c r="L23" s="11" t="n">
+        <f aca="false">L16-L7</f>
+        <v>0.1064</v>
+      </c>
+      <c r="M23" s="12" t="n">
+        <f aca="false">M16-M7</f>
+        <v>0.1227</v>
+      </c>
+      <c r="N23" s="13" t="n">
+        <f aca="false">N16-N7</f>
+        <v>0.02495</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
@@ -2357,8 +2435,18 @@
         <f aca="false">K17-K8</f>
         <v>0.0212</v>
       </c>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
+      <c r="L24" s="15" t="n">
+        <f aca="false">L17-L8</f>
+        <v>0.1462</v>
+      </c>
+      <c r="M24" s="16" t="n">
+        <f aca="false">M17-M8</f>
+        <v>0.1562</v>
+      </c>
+      <c r="N24" s="17" t="n">
+        <f aca="false">N17-N8</f>
+        <v>0.0118</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="28"/>
@@ -6522,7 +6610,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
@@ -6536,12 +6624,14 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L12:N12"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L19:N19"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
   </mergeCells>

</xml_diff>

<commit_message>
Add linear and mlp regressor options
</commit_message>
<xml_diff>
--- a/Plan+Results.xlsx
+++ b/Plan+Results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="119">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -101,13 +101,7 @@
     <t xml:space="preserve">Investigate classification methods: MLP, CNN, RFC, KNN.</t>
   </si>
   <si>
-    <t xml:space="preserve">What's the likelihood one can see a transaction and pick the customer or postcode?</t>
-  </si>
-  <si>
     <t xml:space="preserve">For identifying customer and postcode. On best and worst case scenarios.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What's the likelihood one can see a set of transactions and guess the likelihood?</t>
   </si>
   <si>
     <t xml:space="preserve">Stage 2</t>
@@ -140,6 +134,12 @@
     <t xml:space="preserve">Stage 3 investigates methods to increase privacy and reduce the effectiveness of stage 1 and 2.</t>
   </si>
   <si>
+    <t xml:space="preserve">RMSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
     <t xml:space="preserve">3a</t>
   </si>
   <si>
@@ -149,16 +149,25 @@
     <t xml:space="preserve">1 to n at reasonable intervals</t>
   </si>
   <si>
+    <t xml:space="preserve">Lin Reg</t>
+  </si>
+  <si>
     <t xml:space="preserve">3b</t>
   </si>
   <si>
     <t xml:space="preserve">Transaction obfuscation: random delays and combinations.</t>
   </si>
   <si>
+    <t xml:space="preserve">RF Reg</t>
+  </si>
+  <si>
     <t xml:space="preserve">3c</t>
   </si>
   <si>
     <t xml:space="preserve">Combine best of a and b for a final test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP Reg</t>
   </si>
   <si>
     <t xml:space="preserve">Correl</t>
@@ -470,7 +479,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -548,6 +557,13 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -576,7 +592,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -717,6 +733,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,7 +813,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1145,11 +1169,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="75475290"/>
-        <c:axId val="49332515"/>
+        <c:axId val="91744696"/>
+        <c:axId val="17809391"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75475290"/>
+        <c:axId val="91744696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1229,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49332515"/>
+        <c:crossAx val="17809391"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1213,7 +1237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49332515"/>
+        <c:axId val="17809391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,7 +1302,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75475290"/>
+        <c:crossAx val="91744696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1312,13 +1336,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>87480</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
+      <xdr:colOff>801000</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>171720</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1326,8 +1350,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5249880" y="9319680"/>
-        <a:ext cx="5754960" cy="3234960"/>
+        <a:off x="5249880" y="9293400"/>
+        <a:ext cx="5754240" cy="3234240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1347,8 +1371,8 @@
   </sheetPr>
   <dimension ref="A1:Q316"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N37" activeCellId="0" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2510,34 +2534,28 @@
       <c r="L31" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="0" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="32"/>
       <c r="B32" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L32" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="Q32" s="0" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="32"/>
       <c r="B35" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L35" s="34" t="s">
         <v>20</v>
@@ -2545,10 +2563,10 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L36" s="34" t="s">
         <v>20</v>
@@ -2556,10 +2574,10 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L37" s="34" t="s">
         <v>20</v>
@@ -2570,19 +2588,26 @@
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="32"/>
       <c r="B40" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40" s="35"/>
+      <c r="M40" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="N40" s="36" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="32" t="s">
         <v>38</v>
       </c>
@@ -2592,43 +2617,70 @@
       <c r="H41" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="L41" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="M41" s="35" t="n">
+        <v>0.1571</v>
+      </c>
+      <c r="N41" s="35" t="n">
+        <v>0.7053</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="L42" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="M42" s="35" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="N42" s="35" t="n">
+        <v>0.8166</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="L43" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="M43" s="35" t="n">
+        <v>0.1113</v>
+      </c>
+      <c r="N43" s="35" t="n">
+        <v>0.8507</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="32" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,7 +2691,7 @@
         <v>91</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E47" s="0" t="n">
         <f aca="false">AVERAGE(A47:A316)</f>
@@ -2670,7 +2722,7 @@
         <v>10</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E48" s="0" t="n">
         <f aca="false">AVERAGE(B47:B316)</f>
@@ -6653,7 +6705,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6664,16 +6716,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6696,52 +6748,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="I3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="O3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="U3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12978,7 +13030,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>0.23</v>
@@ -13002,7 +13054,7 @@
         <v>64</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -13022,7 +13074,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>0.26</v>
@@ -13052,7 +13104,7 @@
         <v>73</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -13072,7 +13124,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>0.2</v>
@@ -13102,7 +13154,7 @@
         <v>85</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -19394,17 +19446,17 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S305" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S306" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S307" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -19425,7 +19477,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -19433,16 +19485,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19466,52 +19518,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="I3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="O3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="U3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25748,7 +25800,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -25766,7 +25818,7 @@
         <v>570</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -25786,7 +25838,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -25804,7 +25856,7 @@
         <v>546</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -25824,7 +25876,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -25842,7 +25894,7 @@
         <v>553</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -32134,26 +32186,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -32174,7 +32226,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
@@ -32182,16 +32234,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32215,52 +32267,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="I3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="O3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="U3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38497,7 +38549,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -38515,7 +38567,7 @@
         <v>3360</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -38535,7 +38587,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -38553,7 +38605,7 @@
         <v>3172</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -38573,7 +38625,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -38591,7 +38643,7 @@
         <v>3227</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -44883,26 +44935,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -44923,7 +44975,7 @@
   </sheetPr>
   <dimension ref="A1:W307"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H303" activeCellId="0" sqref="H303"/>
     </sheetView>
   </sheetViews>
@@ -44931,20 +44983,20 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I1" s="0" t="n">
         <f aca="false">COUNTIF(H4:H103,"=1")</f>
         <v>72</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44976,52 +45028,52 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="I3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="O3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Q3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="U3" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51258,7 +51310,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G105" s="0" t="n">
         <v>102</v>
@@ -51276,7 +51328,7 @@
         <v>3281</v>
       </c>
       <c r="M105" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="S105" s="0" t="n">
         <v>102</v>
@@ -51296,7 +51348,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G106" s="0" t="n">
         <v>103</v>
@@ -51314,7 +51366,7 @@
         <v>3285</v>
       </c>
       <c r="M106" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="S106" s="0" t="n">
         <v>103</v>
@@ -51334,7 +51386,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G107" s="0" t="n">
         <v>104</v>
@@ -51352,7 +51404,7 @@
         <v>3161</v>
       </c>
       <c r="M107" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="S107" s="0" t="n">
         <v>104</v>
@@ -57644,26 +57696,26 @@
     </row>
     <row r="305" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G305" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="S305" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G306" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="S306" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G307" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="S307" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>